<commit_message>
changed if multiple samples, but one study
deleted redundant info (study info, smart home, cause and outcome, intervention) and changed code for single_sample and started with scale_number
</commit_message>
<xml_diff>
--- a/data/raw/Review_data_all_packages.xlsx
+++ b/data/raw/Review_data_all_packages.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neleb\Documents\GitHub\CSE-review\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A9D1112-2CAF-4E99-B1D7-2F33D6AD4848}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62D0720B-EC1E-4517-9560-3A36C6B809F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Codebook 1" sheetId="1" r:id="rId1"/>
@@ -10744,13 +10744,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B8C8C23E-B8AC-4554-A9ED-C1B262734E5B}" name="Tabelle1" displayName="Tabelle1" ref="A1:BB185" totalsRowShown="0" headerRowDxfId="98" dataDxfId="97">
-  <autoFilter ref="A1:BB185" xr:uid="{B8C8C23E-B8AC-4554-A9ED-C1B262734E5B}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="43"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:BB185" xr:uid="{B8C8C23E-B8AC-4554-A9ED-C1B262734E5B}"/>
   <tableColumns count="54">
     <tableColumn id="1" xr3:uid="{D02BA947-3664-4909-B808-3612C7EA1856}" name="id" dataDxfId="96"/>
     <tableColumn id="2" xr3:uid="{617FAC16-622B-484B-9C9C-1413492D1A08}" name="publication_type" dataDxfId="95"/>
@@ -10813,13 +10807,7 @@
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabelle2" displayName="Tabelle2" ref="A1:AJ174" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41">
-  <autoFilter ref="A1:AJ174" xr:uid="{00000000-0009-0000-0100-000002000000}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="43"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:AJ174" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="36">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="id" dataDxfId="40"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="authors" dataDxfId="39"/>
@@ -11171,7 +11159,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BB185"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K193" sqref="K193"/>
     </sheetView>
   </sheetViews>
@@ -11393,7 +11381,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>4</v>
       </c>
@@ -11545,7 +11533,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:54" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>10</v>
       </c>
@@ -11703,7 +11691,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>15</v>
       </c>
@@ -11855,7 +11843,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="5" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>19</v>
       </c>
@@ -12007,7 +11995,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>28</v>
       </c>
@@ -12159,7 +12147,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>34</v>
       </c>
@@ -12305,7 +12293,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>42</v>
       </c>
@@ -12457,7 +12445,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>79</v>
       </c>
@@ -12609,7 +12597,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>86</v>
       </c>
@@ -12761,7 +12749,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="11" spans="1:54" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:54" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>95</v>
       </c>
@@ -12904,7 +12892,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="12" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>98</v>
       </c>
@@ -13056,7 +13044,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>111</v>
       </c>
@@ -13208,7 +13196,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>123</v>
       </c>
@@ -13360,7 +13348,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="15" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>124</v>
       </c>
@@ -13515,7 +13503,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="16" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>136</v>
       </c>
@@ -13667,7 +13655,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="17" spans="1:54" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:54" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>157</v>
       </c>
@@ -13819,7 +13807,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="18" spans="1:54" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:54" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>162</v>
       </c>
@@ -13974,7 +13962,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="19" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>164</v>
       </c>
@@ -14126,7 +14114,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:54" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:54" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>173</v>
       </c>
@@ -14281,7 +14269,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="21" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>174</v>
       </c>
@@ -14436,7 +14424,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="22" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>210</v>
       </c>
@@ -14582,7 +14570,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>214</v>
       </c>
@@ -14734,7 +14722,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="24" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>216</v>
       </c>
@@ -14877,7 +14865,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="25" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>219</v>
       </c>
@@ -15029,7 +15017,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="26" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>220</v>
       </c>
@@ -15166,7 +15154,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>233</v>
       </c>
@@ -15318,7 +15306,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>254</v>
       </c>
@@ -15470,7 +15458,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="29" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>263</v>
       </c>
@@ -15613,7 +15601,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="30" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>270</v>
       </c>
@@ -15765,7 +15753,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="31" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>279</v>
       </c>
@@ -15914,7 +15902,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="32" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>312</v>
       </c>
@@ -16057,7 +16045,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="33" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>346</v>
       </c>
@@ -16209,7 +16197,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="34" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>352</v>
       </c>
@@ -16367,7 +16355,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="35" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>355</v>
       </c>
@@ -16519,7 +16507,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="36" spans="1:54" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:54" ht="60" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>362</v>
       </c>
@@ -16671,7 +16659,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="37" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>371</v>
       </c>
@@ -16829,7 +16817,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="38" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>372</v>
       </c>
@@ -16972,7 +16960,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="39" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>372</v>
       </c>
@@ -17115,7 +17103,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="40" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>372</v>
       </c>
@@ -17267,7 +17255,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="41" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>390</v>
       </c>
@@ -17407,7 +17395,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:54" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:54" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>405</v>
       </c>
@@ -17565,7 +17553,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="43" spans="1:54" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:54" ht="75" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>429</v>
       </c>
@@ -17717,7 +17705,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="44" spans="1:54" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:54" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>442</v>
       </c>
@@ -17857,7 +17845,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="45" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>523</v>
       </c>
@@ -17997,7 +17985,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="46" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>527</v>
       </c>
@@ -18152,7 +18140,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="47" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>528</v>
       </c>
@@ -18301,7 +18289,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="48" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>531</v>
       </c>
@@ -18453,7 +18441,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="49" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>533</v>
       </c>
@@ -18605,7 +18593,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="50" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>536</v>
       </c>
@@ -18754,7 +18742,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="51" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>540</v>
       </c>
@@ -18906,7 +18894,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="52" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>550</v>
       </c>
@@ -19052,7 +19040,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="53" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>558</v>
       </c>
@@ -19204,7 +19192,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="54" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>569</v>
       </c>
@@ -19356,7 +19344,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="55" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>569</v>
       </c>
@@ -19508,7 +19496,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="56" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>573</v>
       </c>
@@ -19660,7 +19648,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="57" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>612</v>
       </c>
@@ -19806,7 +19794,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="58" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>676</v>
       </c>
@@ -19958,7 +19946,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="59" spans="1:54" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:54" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>682</v>
       </c>
@@ -20110,7 +20098,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="60" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>690</v>
       </c>
@@ -20253,7 +20241,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="61" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>1</v>
       </c>
@@ -20393,7 +20381,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="62" spans="1:54" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:54" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>11</v>
       </c>
@@ -20551,7 +20539,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>25</v>
       </c>
@@ -20703,7 +20691,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="64" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>36</v>
       </c>
@@ -20846,7 +20834,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="65" spans="1:54" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:54" ht="75" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>56</v>
       </c>
@@ -20995,7 +20983,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="66" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>56</v>
       </c>
@@ -21126,7 +21114,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="67" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>56</v>
       </c>
@@ -21257,7 +21245,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="68" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>56</v>
       </c>
@@ -21388,7 +21376,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="69" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>62</v>
       </c>
@@ -21534,7 +21522,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="70" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>82</v>
       </c>
@@ -21665,7 +21653,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="71" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>87</v>
       </c>
@@ -21814,7 +21802,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="72" spans="1:54" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:54" ht="75" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>94</v>
       </c>
@@ -21954,7 +21942,7 @@
         <v>2190</v>
       </c>
     </row>
-    <row r="73" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>94</v>
       </c>
@@ -22094,7 +22082,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="74" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>94</v>
       </c>
@@ -22234,7 +22222,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="75" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>116</v>
       </c>
@@ -22383,7 +22371,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="76" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>128</v>
       </c>
@@ -22535,7 +22523,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="77" spans="1:54" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:54" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>129</v>
       </c>
@@ -22672,7 +22660,7 @@
         <v>880</v>
       </c>
     </row>
-    <row r="78" spans="1:54" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:54" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>129</v>
       </c>
@@ -22809,7 +22797,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="79" spans="1:54" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:54" ht="30" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>130</v>
       </c>
@@ -22958,7 +22946,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="80" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>147</v>
       </c>
@@ -23107,7 +23095,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="81" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>148</v>
       </c>
@@ -23250,7 +23238,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="82" spans="1:54" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:54" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>155</v>
       </c>
@@ -23396,7 +23384,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="83" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>183</v>
       </c>
@@ -23539,7 +23527,7 @@
         <v>919</v>
       </c>
     </row>
-    <row r="84" spans="1:54" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:54" ht="30" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>188</v>
       </c>
@@ -23682,7 +23670,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="85" spans="1:54" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:54" ht="30" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>200</v>
       </c>
@@ -23834,7 +23822,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="86" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>201</v>
       </c>
@@ -23986,7 +23974,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="87" spans="1:54" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:54" ht="45" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>234</v>
       </c>
@@ -24138,7 +24126,7 @@
         <v>2189</v>
       </c>
     </row>
-    <row r="88" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>242</v>
       </c>
@@ -24290,7 +24278,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="89" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>253</v>
       </c>
@@ -24442,7 +24430,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="90" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>269</v>
       </c>
@@ -24582,7 +24570,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="91" spans="1:54" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:54" ht="30" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>274</v>
       </c>
@@ -24734,7 +24722,7 @@
         <v>985</v>
       </c>
     </row>
-    <row r="92" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>280</v>
       </c>
@@ -24883,7 +24871,7 @@
         <v>919</v>
       </c>
     </row>
-    <row r="93" spans="1:54" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:54" ht="30" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>301</v>
       </c>
@@ -25026,7 +25014,7 @@
         <v>2190</v>
       </c>
     </row>
-    <row r="94" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>325</v>
       </c>
@@ -25175,7 +25163,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="95" spans="1:54" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:54" ht="30" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>335</v>
       </c>
@@ -25312,7 +25300,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="96" spans="1:54" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:54" ht="30" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>337</v>
       </c>
@@ -25461,7 +25449,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="97" spans="1:54" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:54" ht="30" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>339</v>
       </c>
@@ -25613,7 +25601,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="98" spans="1:54" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:54" ht="30" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>367</v>
       </c>
@@ -25762,7 +25750,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="99" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>418</v>
       </c>
@@ -25917,7 +25905,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="100" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>419</v>
       </c>
@@ -26063,7 +26051,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="101" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>465</v>
       </c>
@@ -26209,7 +26197,7 @@
         <v>1070</v>
       </c>
     </row>
-    <row r="102" spans="1:54" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:54" ht="30" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>479</v>
       </c>
@@ -26361,7 +26349,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="103" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>482</v>
       </c>
@@ -26504,7 +26492,7 @@
         <v>1089</v>
       </c>
     </row>
-    <row r="104" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>486</v>
       </c>
@@ -26638,7 +26626,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="105" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>501</v>
       </c>
@@ -26781,7 +26769,7 @@
         <v>2190</v>
       </c>
     </row>
-    <row r="106" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>524</v>
       </c>
@@ -26933,7 +26921,7 @@
         <v>1070</v>
       </c>
     </row>
-    <row r="107" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>553</v>
       </c>
@@ -27082,7 +27070,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="108" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>557</v>
       </c>
@@ -27234,7 +27222,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="109" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>560</v>
       </c>
@@ -27380,7 +27368,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="110" spans="1:54" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:54" ht="30" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>561</v>
       </c>
@@ -27535,7 +27523,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="111" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>600</v>
       </c>
@@ -27681,7 +27669,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="112" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>607</v>
       </c>
@@ -27827,7 +27815,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="113" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>607</v>
       </c>
@@ -27979,7 +27967,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="114" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>627</v>
       </c>
@@ -28125,7 +28113,7 @@
         <v>1070</v>
       </c>
     </row>
-    <row r="115" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>636</v>
       </c>
@@ -28274,7 +28262,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="116" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>650</v>
       </c>
@@ -28426,7 +28414,7 @@
         <v>1181</v>
       </c>
     </row>
-    <row r="117" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>659</v>
       </c>
@@ -28578,7 +28566,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="118" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>660</v>
       </c>
@@ -28730,7 +28718,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="119" spans="1:54" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:54" ht="30" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>675</v>
       </c>
@@ -28879,7 +28867,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="120" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>677</v>
       </c>
@@ -29031,7 +29019,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="121" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>686</v>
       </c>
@@ -29183,7 +29171,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="122" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>687</v>
       </c>
@@ -29329,7 +29317,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="123" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>688</v>
       </c>
@@ -29481,7 +29469,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="124" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>8</v>
       </c>
@@ -29633,7 +29621,7 @@
         <v>2192</v>
       </c>
     </row>
-    <row r="125" spans="1:54" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:54" ht="30" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>26</v>
       </c>
@@ -29785,7 +29773,7 @@
         <v>2190</v>
       </c>
     </row>
-    <row r="126" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>32</v>
       </c>
@@ -30229,7 +30217,7 @@
         <v>2190</v>
       </c>
     </row>
-    <row r="129" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>61</v>
       </c>
@@ -30381,7 +30369,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="130" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>81</v>
       </c>
@@ -30533,7 +30521,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="131" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>83</v>
       </c>
@@ -30679,7 +30667,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="132" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>99</v>
       </c>
@@ -30834,7 +30822,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="133" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>133</v>
       </c>
@@ -30992,7 +30980,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="134" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>146</v>
       </c>
@@ -31144,7 +31132,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="135" spans="1:54" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:54" ht="90" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>150</v>
       </c>
@@ -31293,7 +31281,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="136" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>166</v>
       </c>
@@ -31436,7 +31424,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="137" spans="1:54" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:54" ht="45" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>178</v>
       </c>
@@ -31579,7 +31567,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="138" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>180</v>
       </c>
@@ -31731,7 +31719,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="139" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>180</v>
       </c>
@@ -31883,7 +31871,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="140" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>180</v>
       </c>
@@ -32035,7 +32023,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="141" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>193</v>
       </c>
@@ -32187,7 +32175,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="142" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>236</v>
       </c>
@@ -32342,7 +32330,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="143" spans="1:54" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:54" ht="30" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>248</v>
       </c>
@@ -32494,7 +32482,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="144" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <v>262</v>
       </c>
@@ -32646,7 +32634,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="145" spans="1:54" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:54" ht="30" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>291</v>
       </c>
@@ -32798,7 +32786,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="146" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>302</v>
       </c>
@@ -32950,7 +32938,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="147" spans="1:54" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:54" ht="60" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>303</v>
       </c>
@@ -33099,7 +33087,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="148" spans="1:54" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:54" ht="30" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>324</v>
       </c>
@@ -33248,7 +33236,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="149" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>327</v>
       </c>
@@ -33400,7 +33388,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="150" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>338</v>
       </c>
@@ -33552,7 +33540,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="151" spans="1:54" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:54" ht="30" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <v>342</v>
       </c>
@@ -33704,7 +33692,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="152" spans="1:54" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:54" ht="30" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>347</v>
       </c>
@@ -33850,7 +33838,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="153" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
         <v>348</v>
       </c>
@@ -33990,7 +33978,7 @@
         <v>1581</v>
       </c>
     </row>
-    <row r="154" spans="1:54" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:54" ht="45" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <v>349</v>
       </c>
@@ -34142,7 +34130,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="155" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
         <v>363</v>
       </c>
@@ -34294,7 +34282,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="156" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <v>376</v>
       </c>
@@ -34446,7 +34434,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="157" spans="1:54" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:54" ht="30" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
         <v>378</v>
       </c>
@@ -34598,7 +34586,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="158" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
         <v>381</v>
       </c>
@@ -34741,7 +34729,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="159" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
         <v>384</v>
       </c>
@@ -34887,7 +34875,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="160" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
         <v>400</v>
       </c>
@@ -35039,7 +35027,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="161" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
         <v>408</v>
       </c>
@@ -35191,7 +35179,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="162" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
         <v>408</v>
       </c>
@@ -35331,7 +35319,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="163" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
         <v>412</v>
       </c>
@@ -35483,7 +35471,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="164" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
         <v>430</v>
       </c>
@@ -35632,7 +35620,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="165" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
         <v>433</v>
       </c>
@@ -35784,7 +35772,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="166" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <v>438</v>
       </c>
@@ -35939,7 +35927,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="167" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
         <v>438</v>
       </c>
@@ -36076,7 +36064,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="168" spans="1:54" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:54" ht="30" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
         <v>441</v>
       </c>
@@ -36216,7 +36204,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="169" spans="1:54" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:54" ht="30" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
         <v>452</v>
       </c>
@@ -36362,7 +36350,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="170" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
         <v>497</v>
       </c>
@@ -36511,7 +36499,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="171" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
         <v>498</v>
       </c>
@@ -36660,7 +36648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:54" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:54" ht="30" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
         <v>517</v>
       </c>
@@ -36812,7 +36800,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="173" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
         <v>545</v>
       </c>
@@ -36964,7 +36952,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="174" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
         <v>574</v>
       </c>
@@ -37122,7 +37110,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="175" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
         <v>590</v>
       </c>
@@ -37265,7 +37253,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="176" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
         <v>626</v>
       </c>
@@ -37417,7 +37405,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="177" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
         <v>628</v>
       </c>
@@ -37563,7 +37551,7 @@
         <v>1070</v>
       </c>
     </row>
-    <row r="178" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
         <v>640</v>
       </c>
@@ -37715,7 +37703,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="179" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
         <v>648</v>
       </c>
@@ -37861,7 +37849,7 @@
         <v>1181</v>
       </c>
     </row>
-    <row r="180" spans="1:54" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:54" ht="30" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
         <v>649</v>
       </c>
@@ -38010,7 +37998,7 @@
         <v>1181</v>
       </c>
     </row>
-    <row r="181" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
         <v>672</v>
       </c>
@@ -38165,7 +38153,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="182" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
         <v>678</v>
       </c>
@@ -38317,7 +38305,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="183" spans="1:54" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:54" ht="30" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
         <v>684</v>
       </c>
@@ -38472,7 +38460,7 @@
         <v>1798</v>
       </c>
     </row>
-    <row r="184" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
         <v>685</v>
       </c>
@@ -38627,7 +38615,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="185" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
         <v>689</v>
       </c>
@@ -38793,7 +38781,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AJ174"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="W182" sqref="W182"/>
     </sheetView>
@@ -38941,7 +38929,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="2" spans="1:36" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>4</v>
       </c>
@@ -39043,7 +39031,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:36" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>10</v>
       </c>
@@ -39145,7 +39133,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:36" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:36" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>15</v>
       </c>
@@ -39251,7 +39239,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>19</v>
       </c>
@@ -39351,7 +39339,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:36" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:36" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>28</v>
       </c>
@@ -39457,7 +39445,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:36" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:36" ht="105" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>34</v>
       </c>
@@ -39565,7 +39553,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>42</v>
       </c>
@@ -39663,7 +39651,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:36" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:36" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>79</v>
       </c>
@@ -39773,7 +39761,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:36" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:36" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>86</v>
       </c>
@@ -39875,7 +39863,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>95</v>
       </c>
@@ -39977,7 +39965,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>98</v>
       </c>
@@ -40079,7 +40067,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:36" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:36" ht="135" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>111</v>
       </c>
@@ -40185,7 +40173,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>123</v>
       </c>
@@ -40287,7 +40275,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>136</v>
       </c>
@@ -40391,7 +40379,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:36" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:36" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>157</v>
       </c>
@@ -40501,7 +40489,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:36" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:36" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>162</v>
       </c>
@@ -40609,7 +40597,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:36" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:36" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>164</v>
       </c>
@@ -40719,7 +40707,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:36" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:36" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>173</v>
       </c>
@@ -40825,7 +40813,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>174</v>
       </c>
@@ -40929,7 +40917,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>210</v>
       </c>
@@ -41029,7 +41017,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>214</v>
       </c>
@@ -41131,7 +41119,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:36" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:36" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>216</v>
       </c>
@@ -41237,7 +41225,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>219</v>
       </c>
@@ -41339,7 +41327,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="1:36" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:36" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>220</v>
       </c>
@@ -41447,7 +41435,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>233</v>
       </c>
@@ -41547,7 +41535,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>254</v>
       </c>
@@ -41647,7 +41635,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="1:36" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:36" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>263</v>
       </c>
@@ -41755,7 +41743,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="29" spans="1:36" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:36" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>270</v>
       </c>
@@ -41863,7 +41851,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="30" spans="1:36" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:36" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>279</v>
       </c>
@@ -41965,7 +41953,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="31" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>312</v>
       </c>
@@ -42067,7 +42055,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="32" spans="1:36" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:36" ht="60" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>346</v>
       </c>
@@ -42177,7 +42165,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="33" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>352</v>
       </c>
@@ -42281,7 +42269,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="34" spans="1:36" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:36" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>355</v>
       </c>
@@ -42387,7 +42375,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="35" spans="1:36" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:36" ht="90" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>362</v>
       </c>
@@ -42491,7 +42479,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="36" spans="1:36" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:36" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>371</v>
       </c>
@@ -42597,7 +42585,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="37" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>372</v>
       </c>
@@ -42695,7 +42683,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="38" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>372</v>
       </c>
@@ -42793,7 +42781,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="39" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>372</v>
       </c>
@@ -42895,7 +42883,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="40" spans="1:36" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:36" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>405</v>
       </c>
@@ -43001,7 +42989,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:36" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:36" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>429</v>
       </c>
@@ -43105,7 +43093,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>442</v>
       </c>
@@ -43207,7 +43195,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="43" spans="1:36" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:36" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>523</v>
       </c>
@@ -43315,7 +43303,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="44" spans="1:36" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:36" ht="90" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>528</v>
       </c>
@@ -43421,7 +43409,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="45" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>531</v>
       </c>
@@ -43523,7 +43511,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="46" spans="1:36" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:36" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>533</v>
       </c>
@@ -43629,7 +43617,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="47" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>536</v>
       </c>
@@ -43725,7 +43713,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="48" spans="1:36" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:36" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>540</v>
       </c>
@@ -43835,7 +43823,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="49" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>550</v>
       </c>
@@ -43937,7 +43925,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="50" spans="1:36" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:36" ht="60" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>558</v>
       </c>
@@ -44043,7 +44031,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="51" spans="1:36" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:36" ht="45" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>569</v>
       </c>
@@ -44147,7 +44135,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="52" spans="1:36" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:36" ht="75" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>573</v>
       </c>
@@ -44251,7 +44239,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="53" spans="1:36" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:36" ht="90" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>676</v>
       </c>
@@ -44359,7 +44347,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="54" spans="1:36" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:36" ht="60" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>682</v>
       </c>
@@ -44463,7 +44451,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="55" spans="1:36" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:36" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>690</v>
       </c>
@@ -44563,7 +44551,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="56" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>1</v>
       </c>
@@ -44663,7 +44651,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="57" spans="1:36" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:36" ht="60" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>11</v>
       </c>
@@ -44769,7 +44757,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="58" spans="1:36" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:36" ht="90" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>25</v>
       </c>
@@ -44871,7 +44859,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="59" spans="1:36" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:36" ht="60" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>36</v>
       </c>
@@ -44979,7 +44967,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="60" spans="1:36" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:36" ht="135" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>56</v>
       </c>
@@ -45087,7 +45075,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="61" spans="1:36" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:36" ht="135" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>56</v>
       </c>
@@ -45193,7 +45181,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="62" spans="1:36" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:36" ht="135" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>56</v>
       </c>
@@ -45299,7 +45287,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="63" spans="1:36" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:36" ht="135" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>56</v>
       </c>
@@ -45405,7 +45393,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="64" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -45503,7 +45491,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="65" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>82</v>
       </c>
@@ -45597,7 +45585,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="66" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>87</v>
       </c>
@@ -45695,7 +45683,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="67" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>94</v>
       </c>
@@ -45799,7 +45787,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="68" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>94</v>
       </c>
@@ -45903,7 +45891,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="69" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>94</v>
       </c>
@@ -46007,7 +45995,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="70" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>116</v>
       </c>
@@ -46109,7 +46097,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="71" spans="1:36" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:36" ht="30" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>128</v>
       </c>
@@ -46219,7 +46207,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="72" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>129</v>
       </c>
@@ -46321,7 +46309,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="73" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>129</v>
       </c>
@@ -46423,7 +46411,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="74" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>130</v>
       </c>
@@ -46525,7 +46513,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="75" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>147</v>
       </c>
@@ -46625,7 +46613,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="76" spans="1:36" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:36" ht="60" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>148</v>
       </c>
@@ -46729,7 +46717,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="77" spans="1:36" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:36" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>155</v>
       </c>
@@ -46829,7 +46817,7 @@
       <c r="AI77" s="1"/>
       <c r="AJ77" s="1"/>
     </row>
-    <row r="78" spans="1:36" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:36" ht="60" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>183</v>
       </c>
@@ -46927,7 +46915,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="79" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>188</v>
       </c>
@@ -47027,7 +47015,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="80" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>200</v>
       </c>
@@ -47133,7 +47121,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="81" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>201</v>
       </c>
@@ -47231,7 +47219,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="82" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>234</v>
       </c>
@@ -47333,7 +47321,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="83" spans="1:36" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:36" ht="60" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>242</v>
       </c>
@@ -47439,7 +47427,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="84" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>253</v>
       </c>
@@ -47537,7 +47525,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="85" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>269</v>
       </c>
@@ -47635,7 +47623,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="86" spans="1:36" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:36" ht="75" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>274</v>
       </c>
@@ -47739,7 +47727,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="87" spans="1:36" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:36" ht="45" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>280</v>
       </c>
@@ -47843,7 +47831,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="88" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>301</v>
       </c>
@@ -47941,7 +47929,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="89" spans="1:36" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:36" ht="135" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>325</v>
       </c>
@@ -48049,7 +48037,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="90" spans="1:36" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:36" ht="45" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>335</v>
       </c>
@@ -48155,7 +48143,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="91" spans="1:36" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:36" ht="75" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>337</v>
       </c>
@@ -48257,7 +48245,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="92" spans="1:36" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:36" ht="60" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>339</v>
       </c>
@@ -48363,7 +48351,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="93" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>367</v>
       </c>
@@ -48467,7 +48455,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="94" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>418</v>
       </c>
@@ -48565,7 +48553,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="95" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>419</v>
       </c>
@@ -48667,7 +48655,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="96" spans="1:36" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:36" ht="45" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>465</v>
       </c>
@@ -48769,7 +48757,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="97" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>479</v>
       </c>
@@ -48871,7 +48859,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="98" spans="1:36" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:36" ht="90" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>482</v>
       </c>
@@ -48969,7 +48957,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="99" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>486</v>
       </c>
@@ -49069,7 +49057,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="100" spans="1:36" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:36" ht="30" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>501</v>
       </c>
@@ -49177,7 +49165,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="101" spans="1:36" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:36" ht="30" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>524</v>
       </c>
@@ -49281,7 +49269,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="102" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>553</v>
       </c>
@@ -49383,7 +49371,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="103" spans="1:36" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:36" ht="60" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>557</v>
       </c>
@@ -49487,7 +49475,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="104" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>560</v>
       </c>
@@ -49591,7 +49579,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="105" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>561</v>
       </c>
@@ -49697,7 +49685,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="106" spans="1:36" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:36" ht="45" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>600</v>
       </c>
@@ -49797,7 +49785,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="107" spans="1:36" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:36" ht="45" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>627</v>
       </c>
@@ -49905,7 +49893,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="108" spans="1:36" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:36" ht="90" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>636</v>
       </c>
@@ -50007,7 +49995,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="109" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>650</v>
       </c>
@@ -50105,7 +50093,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="110" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>659</v>
       </c>
@@ -50203,7 +50191,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="111" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>660</v>
       </c>
@@ -50307,7 +50295,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="112" spans="1:36" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:36" ht="45" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>675</v>
       </c>
@@ -50415,7 +50403,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="113" spans="1:36" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:36" ht="75" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>677</v>
       </c>
@@ -50511,7 +50499,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="114" spans="1:36" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:36" ht="45" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>686</v>
       </c>
@@ -50613,7 +50601,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="115" spans="1:36" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:36" ht="75" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>687</v>
       </c>
@@ -50717,7 +50705,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="116" spans="1:36" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:36" ht="30" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>688</v>
       </c>
@@ -50825,7 +50813,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="117" spans="1:36" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:36" ht="45" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>8</v>
       </c>
@@ -50933,7 +50921,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="118" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>26</v>
       </c>
@@ -51037,7 +51025,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="119" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>32</v>
       </c>
@@ -51351,7 +51339,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="122" spans="1:36" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:36" ht="75" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>61</v>
       </c>
@@ -51461,7 +51449,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="123" spans="1:36" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:36" ht="45" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>81</v>
       </c>
@@ -51569,7 +51557,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="124" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>83</v>
       </c>
@@ -51667,7 +51655,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="125" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>99</v>
       </c>
@@ -51755,7 +51743,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="126" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>133</v>
       </c>
@@ -51857,7 +51845,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="127" spans="1:36" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:36" ht="30" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>146</v>
       </c>
@@ -51965,7 +51953,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="128" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>150</v>
       </c>
@@ -52071,7 +52059,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="129" spans="1:36" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:36" ht="165" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>166</v>
       </c>
@@ -52181,7 +52169,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="130" spans="1:36" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:36" ht="60" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>178</v>
       </c>
@@ -52283,7 +52271,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="131" spans="1:36" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:36" ht="45" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>180</v>
       </c>
@@ -52393,7 +52381,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="132" spans="1:36" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:36" ht="45" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>180</v>
       </c>
@@ -52503,7 +52491,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="133" spans="1:36" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:36" ht="45" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>180</v>
       </c>
@@ -52611,7 +52599,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="134" spans="1:36" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:36" ht="60" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>193</v>
       </c>
@@ -52719,7 +52707,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="135" spans="1:36" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:36" ht="60" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>236</v>
       </c>
@@ -52825,7 +52813,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="136" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>248</v>
       </c>
@@ -52923,7 +52911,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="137" spans="1:36" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:36" ht="30" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>262</v>
       </c>
@@ -53031,7 +53019,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="138" spans="1:36" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:36" ht="75" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>291</v>
       </c>
@@ -53139,7 +53127,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="139" spans="1:36" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:36" ht="45" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>302</v>
       </c>
@@ -53247,7 +53235,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="140" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>303</v>
       </c>
@@ -53349,7 +53337,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="141" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>324</v>
       </c>
@@ -53453,7 +53441,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="142" spans="1:36" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:36" ht="60" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>327</v>
       </c>
@@ -53555,7 +53543,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="143" spans="1:36" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:36" ht="60" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>338</v>
       </c>
@@ -53657,7 +53645,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="144" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <v>342</v>
       </c>
@@ -53763,7 +53751,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="145" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>347</v>
       </c>
@@ -53855,7 +53843,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="146" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>348</v>
       </c>
@@ -53959,7 +53947,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="147" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>349</v>
       </c>
@@ -54065,7 +54053,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="148" spans="1:36" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:36" ht="45" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>363</v>
       </c>
@@ -54173,7 +54161,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="149" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>376</v>
       </c>
@@ -54277,7 +54265,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="150" spans="1:36" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:36" ht="90" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>378</v>
       </c>
@@ -54385,7 +54373,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="151" spans="1:36" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:36" ht="30" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <v>381</v>
       </c>
@@ -54487,7 +54475,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="152" spans="1:36" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:36" ht="75" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>384</v>
       </c>
@@ -54595,7 +54583,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="153" spans="1:36" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:36" ht="120" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
         <v>400</v>
       </c>
@@ -54701,7 +54689,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="154" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <v>408</v>
       </c>
@@ -54807,7 +54795,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="155" spans="1:36" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:36" ht="75" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
         <v>412</v>
       </c>
@@ -54913,7 +54901,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="156" spans="1:36" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:36" ht="45" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <v>430</v>
       </c>
@@ -55015,7 +55003,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="157" spans="1:36" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:36" ht="60" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
         <v>433</v>
       </c>
@@ -55121,7 +55109,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="158" spans="1:36" s="3" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:36" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
         <v>438</v>
       </c>
@@ -55231,7 +55219,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="159" spans="1:36" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:36" ht="60" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
         <v>441</v>
       </c>
@@ -55307,7 +55295,7 @@
       <c r="AI159" s="1"/>
       <c r="AJ159" s="1"/>
     </row>
-    <row r="160" spans="1:36" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:36" ht="60" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
         <v>452</v>
       </c>
@@ -55413,7 +55401,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="161" spans="1:36" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:36" ht="45" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
         <v>497</v>
       </c>
@@ -55517,7 +55505,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="162" spans="1:36" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:36" ht="30" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
         <v>498</v>
       </c>
@@ -55625,7 +55613,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="163" spans="1:36" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:36" ht="75" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
         <v>517</v>
       </c>
@@ -55735,7 +55723,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="164" spans="1:36" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:36" ht="45" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
         <v>545</v>
       </c>
@@ -55839,7 +55827,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="165" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
         <v>574</v>
       </c>
@@ -55943,7 +55931,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="166" spans="1:36" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:36" ht="60" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <v>590</v>
       </c>
@@ -56049,7 +56037,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="167" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
         <v>626</v>
       </c>
@@ -56151,7 +56139,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="168" spans="1:36" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:36" ht="45" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
         <v>628</v>
       </c>
@@ -56261,7 +56249,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="169" spans="1:36" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:36" ht="60" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
         <v>640</v>
       </c>
@@ -56369,7 +56357,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="170" spans="1:36" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:36" ht="60" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
         <v>672</v>
       </c>
@@ -56477,7 +56465,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="171" spans="1:36" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:36" ht="75" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
         <v>678</v>
       </c>
@@ -56583,7 +56571,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="172" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
         <v>684</v>
       </c>
@@ -56689,7 +56677,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="173" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
         <v>685</v>
       </c>
@@ -56795,7 +56783,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="174" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
         <v>689</v>
       </c>

</xml_diff>

<commit_message>
updated content validity expert column
</commit_message>
<xml_diff>
--- a/data/raw/Review_data_all_packages.xlsx
+++ b/data/raw/Review_data_all_packages.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neleb\Documents\GitHub\CSE-review\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63781AD2-AAAE-47F7-9E51-6FC22BECEB9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{966510F5-E3AC-44BA-95BC-5A49ECA44BA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Codebook 1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9849" uniqueCount="2796">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9845" uniqueCount="2794">
   <si>
     <t>id</t>
   </si>
@@ -8948,12 +8948,6 @@
   </si>
   <si>
     <t>validity_content_experts: coded by only one coder. 0 = no mention of expert consultation; 1 = experts consulted</t>
-  </si>
-  <si>
-    <t>1?</t>
-  </si>
-  <si>
-    <t>0?</t>
   </si>
 </sst>
 </file>
@@ -39369,7 +39363,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="U1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="W3" sqref="W3"/>
+      <selection pane="topRight" activeCell="X3" sqref="X3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -43105,7 +43099,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="36" spans="1:37" ht="135" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:37" ht="390" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>111</v>
       </c>
@@ -43168,11 +43162,11 @@
       <c r="V36" s="1">
         <v>1</v>
       </c>
-      <c r="W36" s="1" t="s">
+      <c r="W36" s="2" t="s">
         <v>2310</v>
       </c>
-      <c r="X36" s="1" t="s">
-        <v>2794</v>
+      <c r="X36" s="1">
+        <v>1</v>
       </c>
       <c r="Y36" s="1">
         <v>2</v>
@@ -48203,7 +48197,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="84" spans="1:37" ht="75" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:37" ht="90" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>291</v>
       </c>
@@ -48268,11 +48262,11 @@
       <c r="V84" s="1">
         <v>1</v>
       </c>
-      <c r="W84" s="1" t="s">
+      <c r="W84" s="2" t="s">
         <v>2331</v>
       </c>
-      <c r="X84" s="1" t="s">
-        <v>2795</v>
+      <c r="X84" s="1">
+        <v>1</v>
       </c>
       <c r="Y84" s="1" t="s">
         <v>39</v>
@@ -53037,7 +53031,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="130" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:37" ht="165" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>486</v>
       </c>
@@ -53100,11 +53094,11 @@
       <c r="V130" s="1">
         <v>1</v>
       </c>
-      <c r="W130" s="1" t="s">
+      <c r="W130" s="2" t="s">
         <v>2326</v>
       </c>
-      <c r="X130" s="1" t="s">
-        <v>2794</v>
+      <c r="X130" s="1">
+        <v>1</v>
       </c>
       <c r="Y130" s="1"/>
       <c r="Z130" s="1"/>
@@ -53140,7 +53134,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="131" spans="1:37" ht="45" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:37" ht="225" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>497</v>
       </c>
@@ -53201,11 +53195,11 @@
       <c r="V131" s="1">
         <v>1</v>
       </c>
-      <c r="W131" s="1" t="s">
+      <c r="W131" s="2" t="s">
         <v>1929</v>
       </c>
-      <c r="X131" s="1" t="s">
-        <v>2795</v>
+      <c r="X131" s="1">
+        <v>0</v>
       </c>
       <c r="Y131" s="1" t="s">
         <v>39</v>

</xml_diff>

<commit_message>
updated analysis regarding factor validity
</commit_message>
<xml_diff>
--- a/data/raw/Review_data_all_packages.xlsx
+++ b/data/raw/Review_data_all_packages.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neleb\Documents\GitHub\CSE-review\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98FA2914-34CF-4BA6-B0EA-3A189F812C03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6306F8B-B6F2-4F05-947F-BA5B1115102A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="15585" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Codebook 1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9844" uniqueCount="2793">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9832" uniqueCount="2798">
   <si>
     <t>id</t>
   </si>
@@ -8945,6 +8945,21 @@
   </si>
   <si>
     <t>validity_content_experts: coded by only one coder. 0 = no mention of expert consultation; 1 = experts consulted</t>
+  </si>
+  <si>
+    <t>factor validity (CFA, unidimensional constructs)</t>
+  </si>
+  <si>
+    <t>X2 (136) = 1,767.65, p = .001</t>
+  </si>
+  <si>
+    <t>Construct Validity and Reliability: The 17 items used to measure the different constructs of the study were subjected to a principal component analysis; Kaiser-Meyer Olkin Measure of Sampling Adequacy was pegged at 82; Bartlett’s Test of Sphericity [X2 (136) = 1,767.65, p = .001] indicated that the correlations among the 17 items; Eigenvalues for the five components were higher than the Kaiser’s criterion of 1 (values ranging from 4.74 to 1.11) and in combination accounted for 65.83% of the variance; Table 2 shows the factor loadings of the 17 items</t>
+  </si>
+  <si>
+    <t>Exploratory factor analyses were used to assess convergent and discriminant validity: All eigenvalues associated with the factors exceeded the required level of 1.0, varying from 1.14 to 3.73; As shown in Table 1, the overall factor structural solution had an appropriate loading pattern and explained 68.94 percent of the variation.</t>
+  </si>
+  <si>
+    <t>no specific reporting</t>
   </si>
 </sst>
 </file>
@@ -9021,7 +9036,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -9044,6 +9059,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -10854,9 +10870,15 @@
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabelle2" displayName="Tabelle2" ref="A1:AK174" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42">
-  <autoFilter ref="A1:AK174" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AK174">
-    <sortCondition ref="A1:A174"/>
+  <autoFilter ref="A1:AK174" xr:uid="{00000000-0009-0000-0100-000002000000}">
+    <filterColumn colId="12">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A25:AK163">
+    <sortCondition ref="Z1:Z174"/>
   </sortState>
   <tableColumns count="37">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="id" dataDxfId="41"/>
@@ -11210,8 +11232,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BC185"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView topLeftCell="U1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AB11" sqref="AB11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11243,7 +11265,7 @@
     <col min="26" max="26" width="33" style="1" customWidth="1"/>
     <col min="27" max="27" width="28.5703125" style="1" customWidth="1"/>
     <col min="28" max="28" width="63.85546875" style="1" customWidth="1"/>
-    <col min="29" max="29" width="22" style="1" customWidth="1"/>
+    <col min="29" max="29" width="71.28515625" style="1" customWidth="1"/>
     <col min="30" max="30" width="63.28515625" style="2" customWidth="1"/>
     <col min="31" max="31" width="31.7109375" style="1" customWidth="1"/>
     <col min="32" max="34" width="21.28515625" style="1" customWidth="1"/>
@@ -13141,7 +13163,7 @@
         <v>779</v>
       </c>
     </row>
-    <row r="13" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:55" ht="90" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>34</v>
       </c>
@@ -13226,7 +13248,7 @@
       <c r="AB13" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AC13" s="1" t="s">
+      <c r="AC13" s="2" t="s">
         <v>2033</v>
       </c>
       <c r="AD13" s="1">
@@ -19149,7 +19171,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="53" spans="1:55" ht="30" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:55" ht="120" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>164</v>
       </c>
@@ -19234,7 +19256,7 @@
       <c r="AB53" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="AC53" s="1" t="s">
+      <c r="AC53" s="2" t="s">
         <v>2497</v>
       </c>
       <c r="AD53" s="1">
@@ -19693,7 +19715,7 @@
       <c r="AB56" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AC56" s="1" t="s">
+      <c r="AC56" s="2" t="s">
         <v>2029</v>
       </c>
       <c r="AD56" s="1">
@@ -21136,7 +21158,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="66" spans="1:55" ht="30" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:55" ht="60" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>210</v>
       </c>
@@ -21215,7 +21237,7 @@
       <c r="AB66" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AC66" s="1" t="s">
+      <c r="AC66" s="2" t="s">
         <v>2030</v>
       </c>
       <c r="AD66" s="1">
@@ -21672,7 +21694,7 @@
       <c r="AB69" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AC69" s="1" t="s">
+      <c r="AC69" s="2" t="s">
         <v>2031</v>
       </c>
       <c r="AD69" s="1">
@@ -31902,7 +31924,7 @@
       </c>
       <c r="BC136" s="1"/>
     </row>
-    <row r="137" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:55" ht="60" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>501</v>
       </c>
@@ -31984,7 +32006,7 @@
       <c r="AB137" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AC137" s="1" t="s">
+      <c r="AC137" s="2" t="s">
         <v>2032</v>
       </c>
       <c r="AD137" s="1">
@@ -32502,7 +32524,7 @@
         <v>1067</v>
       </c>
     </row>
-    <row r="141" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:55" ht="165" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>527</v>
       </c>
@@ -32587,7 +32609,7 @@
       <c r="AB141" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AC141" s="1" t="s">
+      <c r="AC141" s="2" t="s">
         <v>2034</v>
       </c>
       <c r="AD141" s="1">
@@ -35396,7 +35418,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="160" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:55" ht="75" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
         <v>607</v>
       </c>
@@ -35481,7 +35503,7 @@
       <c r="AB160" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AC160" s="1" t="s">
+      <c r="AC160" s="2" t="s">
         <v>2035</v>
       </c>
       <c r="AD160" s="1">
@@ -39358,9 +39380,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AK174"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="U1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Z7" sqref="Z7"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="X1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AA163" sqref="AA163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -39510,7 +39532,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -39613,7 +39635,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:37" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:37" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>4</v>
       </c>
@@ -39716,7 +39738,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:37" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:37" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>8</v>
       </c>
@@ -39827,7 +39849,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:37" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:37" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>10</v>
       </c>
@@ -39932,7 +39954,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:37" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:37" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>11</v>
       </c>
@@ -40041,7 +40063,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:37" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:37" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>15</v>
       </c>
@@ -40150,7 +40172,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>19</v>
       </c>
@@ -40253,7 +40275,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:37" ht="90" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:37" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>25</v>
       </c>
@@ -40358,7 +40380,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>26</v>
       </c>
@@ -40465,7 +40487,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:37" ht="60" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:37" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>28</v>
       </c>
@@ -40574,7 +40596,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>32</v>
       </c>
@@ -40683,7 +40705,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:37" ht="105" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:37" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>34</v>
       </c>
@@ -40794,7 +40816,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:37" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:37" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>36</v>
       </c>
@@ -40903,7 +40925,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>42</v>
       </c>
@@ -41004,7 +41026,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>43</v>
       </c>
@@ -41113,7 +41135,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>43</v>
       </c>
@@ -41218,7 +41240,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:37" ht="135" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:37" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>56</v>
       </c>
@@ -41329,7 +41351,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:37" ht="135" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:37" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>56</v>
       </c>
@@ -41436,7 +41458,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:37" ht="135" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:37" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>56</v>
       </c>
@@ -41543,7 +41565,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:37" ht="135" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:37" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>56</v>
       </c>
@@ -41650,7 +41672,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:37" ht="75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:37" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>61</v>
       </c>
@@ -41761,7 +41783,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>62</v>
       </c>
@@ -41860,7 +41882,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:37" ht="60" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:37" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>79</v>
       </c>
@@ -41973,58 +41995,56 @@
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="1:37" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:37" ht="75" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>81</v>
+        <v>98</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>1413</v>
+        <v>137</v>
       </c>
       <c r="C25" s="1">
-        <v>2016</v>
-      </c>
-      <c r="D25" s="1">
-        <v>7</v>
+        <v>2019</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>145</v>
       </c>
       <c r="E25" s="1">
-        <v>112</v>
+        <v>11</v>
       </c>
       <c r="F25" s="1">
         <v>1</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>1827</v>
+        <v>647</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>1828</v>
+        <v>648</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>2229</v>
+        <v>2222</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>2251</v>
+        <v>649</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>727</v>
+        <v>605</v>
       </c>
       <c r="L25" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M25" s="1">
         <v>1</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>1829</v>
+        <v>39</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>1830</v>
+        <v>39</v>
       </c>
       <c r="P25" s="1" t="s">
-        <v>1831</v>
-      </c>
-      <c r="Q25" s="6">
-        <v>0.73</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="Q25" s="6"/>
       <c r="R25" s="1" t="s">
         <v>39</v>
       </c>
@@ -42036,44 +42056,38 @@
         <v>39</v>
       </c>
       <c r="V25" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W25" s="1" t="s">
-        <v>1832</v>
-      </c>
-      <c r="X25" s="1">
-        <v>0</v>
-      </c>
-      <c r="Y25" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z25" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AA25" s="1" t="s">
-        <v>39</v>
+        <v>39</v>
+      </c>
+      <c r="X25" s="1"/>
+      <c r="Y25" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z25" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA25" s="2" t="s">
+        <v>2382</v>
       </c>
       <c r="AB25" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AC25" s="1">
-        <v>5</v>
+      <c r="AC25" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="AD25" s="1" t="s">
-        <v>2447</v>
-      </c>
-      <c r="AE25" s="2" t="s">
-        <v>2746</v>
-      </c>
-      <c r="AF25" s="1">
-        <v>5</v>
+        <v>39</v>
+      </c>
+      <c r="AE25" s="2"/>
+      <c r="AF25" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="AG25" s="1" t="s">
-        <v>2447</v>
-      </c>
-      <c r="AH25" s="2" t="s">
-        <v>2746</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="AH25" s="10"/>
       <c r="AI25" s="1" t="s">
         <v>39</v>
       </c>
@@ -42084,7 +42098,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>82</v>
       </c>
@@ -42181,7 +42195,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>83</v>
       </c>
@@ -42280,7 +42294,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="1:37" ht="60" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:37" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>86</v>
       </c>
@@ -42385,7 +42399,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="29" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>87</v>
       </c>
@@ -42486,7 +42500,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="30" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>94</v>
       </c>
@@ -42591,7 +42605,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="31" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>94</v>
       </c>
@@ -42696,7 +42710,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="32" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>94</v>
       </c>
@@ -42801,7 +42815,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="33" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>95</v>
       </c>
@@ -42904,42 +42918,42 @@
         <v>39</v>
       </c>
     </row>
-    <row r="34" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:37" ht="60" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>98</v>
+        <v>162</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>137</v>
+        <v>201</v>
       </c>
       <c r="C34" s="1">
-        <v>2019</v>
+        <v>2015</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>145</v>
+        <v>207</v>
       </c>
       <c r="E34" s="1">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="F34" s="1">
         <v>1</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>647</v>
+        <v>668</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>648</v>
+        <v>669</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>2222</v>
+        <v>1906</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>649</v>
+        <v>644</v>
       </c>
       <c r="K34" s="1" t="s">
         <v>605</v>
       </c>
       <c r="L34" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="M34" s="1">
         <v>1</v>
@@ -42948,12 +42962,14 @@
         <v>39</v>
       </c>
       <c r="O34" s="1" t="s">
-        <v>39</v>
+        <v>670</v>
       </c>
       <c r="P34" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q34" s="6"/>
+        <v>671</v>
+      </c>
+      <c r="Q34" s="7">
+        <v>0.79</v>
+      </c>
       <c r="R34" s="1" t="s">
         <v>39</v>
       </c>
@@ -42965,38 +42981,44 @@
         <v>39</v>
       </c>
       <c r="V34" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W34" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="X34" s="1"/>
+        <v>2311</v>
+      </c>
+      <c r="X34" s="1">
+        <v>0</v>
+      </c>
       <c r="Y34" s="1">
         <v>0</v>
       </c>
       <c r="Z34" s="1">
         <v>0</v>
       </c>
-      <c r="AA34" s="1" t="s">
-        <v>2382</v>
+      <c r="AA34" s="2" t="s">
+        <v>2384</v>
       </c>
       <c r="AB34" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AC34" s="1" t="s">
-        <v>39</v>
+      <c r="AC34" s="1">
+        <v>5</v>
       </c>
       <c r="AD34" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AE34" s="2"/>
-      <c r="AF34" s="1" t="s">
-        <v>39</v>
+        <v>2385</v>
+      </c>
+      <c r="AE34" s="2" t="s">
+        <v>2699</v>
+      </c>
+      <c r="AF34" s="1">
+        <v>4</v>
       </c>
       <c r="AG34" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AH34" s="10"/>
+        <v>2386</v>
+      </c>
+      <c r="AH34" s="10" t="s">
+        <v>2699</v>
+      </c>
       <c r="AI34" s="1" t="s">
         <v>39</v>
       </c>
@@ -43007,7 +43029,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="35" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>99</v>
       </c>
@@ -43096,59 +43118,61 @@
         <v>39</v>
       </c>
     </row>
-    <row r="36" spans="1:37" ht="390" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:37" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>111</v>
+        <v>501</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>148</v>
+        <v>1093</v>
       </c>
       <c r="C36" s="1">
-        <v>2010</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>153</v>
+        <v>2020</v>
+      </c>
+      <c r="D36" s="1">
+        <v>39</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>877</v>
-      </c>
-      <c r="F36" s="1">
-        <v>0</v>
-      </c>
+        <v>2198</v>
+      </c>
+      <c r="F36" s="1"/>
       <c r="G36" s="1" t="s">
-        <v>39</v>
+        <v>1331</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I36" s="1"/>
+        <v>626</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>626</v>
+      </c>
       <c r="J36" s="1" t="s">
-        <v>650</v>
+        <v>731</v>
       </c>
       <c r="K36" s="1" t="s">
         <v>605</v>
       </c>
       <c r="L36" s="1">
-        <v>3</v>
-      </c>
-      <c r="M36" s="1" t="s">
-        <v>39</v>
+        <v>2</v>
+      </c>
+      <c r="M36" s="1">
+        <v>1</v>
       </c>
       <c r="N36" s="1" t="s">
         <v>39</v>
       </c>
       <c r="O36" s="1" t="s">
-        <v>651</v>
+        <v>2285</v>
       </c>
       <c r="P36" s="1" t="s">
-        <v>652</v>
-      </c>
-      <c r="Q36" s="6"/>
+        <v>1097</v>
+      </c>
+      <c r="Q36" s="6">
+        <v>0.79</v>
+      </c>
       <c r="R36" s="1" t="s">
-        <v>653</v>
+        <v>1097</v>
       </c>
       <c r="S36" s="1">
-        <v>0.98199999999999998</v>
+        <v>0.79</v>
       </c>
       <c r="T36" s="1" t="s">
         <v>39</v>
@@ -43157,22 +43181,20 @@
         <v>39</v>
       </c>
       <c r="V36" s="1">
-        <v>1</v>
-      </c>
-      <c r="W36" s="2" t="s">
-        <v>2310</v>
-      </c>
-      <c r="X36" s="1">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="W36" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="X36" s="1"/>
       <c r="Y36" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Z36" s="1">
-        <v>2</v>
-      </c>
-      <c r="AA36" s="1" t="s">
-        <v>2341</v>
+        <v>0</v>
+      </c>
+      <c r="AA36" s="2" t="s">
+        <v>1332</v>
       </c>
       <c r="AB36" s="1" t="s">
         <v>39</v>
@@ -43181,19 +43203,19 @@
         <v>5</v>
       </c>
       <c r="AD36" s="1" t="s">
-        <v>2501</v>
+        <v>1333</v>
       </c>
       <c r="AE36" s="2" t="s">
-        <v>2723</v>
-      </c>
-      <c r="AF36" s="1">
-        <v>3</v>
+        <v>2357</v>
+      </c>
+      <c r="AF36" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="AG36" s="1" t="s">
-        <v>2502</v>
-      </c>
-      <c r="AH36" s="10" t="s">
-        <v>2723</v>
+        <v>39</v>
+      </c>
+      <c r="AH36" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="AI36" s="1" t="s">
         <v>39</v>
@@ -43205,7 +43227,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="37" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>116</v>
       </c>
@@ -43308,60 +43330,64 @@
         <v>39</v>
       </c>
     </row>
-    <row r="38" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:37" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>123</v>
+        <v>540</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>157</v>
+        <v>492</v>
       </c>
       <c r="C38" s="1">
-        <v>2016</v>
+        <v>2018</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="E38" s="1">
-        <v>13</v>
+        <v>497</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>2183</v>
       </c>
       <c r="F38" s="1">
+        <v>2</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>751</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>752</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>703</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="K38" s="1" t="s">
+        <v>753</v>
+      </c>
+      <c r="L38" s="1">
         <v>3</v>
       </c>
-      <c r="G38" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H38" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I38" s="1"/>
-      <c r="J38" s="1" t="s">
-        <v>2233</v>
-      </c>
-      <c r="K38" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="L38" s="1">
-        <v>35</v>
-      </c>
       <c r="M38" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="N38" s="1" t="s">
-        <v>654</v>
+        <v>39</v>
       </c>
       <c r="O38" s="1" t="s">
-        <v>655</v>
+        <v>754</v>
       </c>
       <c r="P38" s="1" t="s">
-        <v>656</v>
+        <v>755</v>
       </c>
       <c r="Q38" s="1">
-        <v>0.97499999999999998</v>
+        <v>0.85</v>
       </c>
       <c r="R38" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="S38" s="1"/>
+        <v>756</v>
+      </c>
+      <c r="S38" s="1">
+        <v>0.86</v>
+      </c>
       <c r="T38" s="1" t="s">
         <v>39</v>
       </c>
@@ -43372,7 +43398,7 @@
         <v>1</v>
       </c>
       <c r="W38" s="1" t="s">
-        <v>657</v>
+        <v>2319</v>
       </c>
       <c r="X38" s="1">
         <v>0</v>
@@ -43383,26 +43409,30 @@
       <c r="Z38" s="1">
         <v>0</v>
       </c>
-      <c r="AA38" s="1" t="s">
-        <v>2383</v>
+      <c r="AA38" s="2" t="s">
+        <v>2409</v>
       </c>
       <c r="AB38" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AC38" s="1" t="s">
-        <v>39</v>
+      <c r="AC38" s="1">
+        <v>5</v>
       </c>
       <c r="AD38" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AE38" s="2"/>
-      <c r="AF38" s="1" t="s">
-        <v>39</v>
+        <v>2410</v>
+      </c>
+      <c r="AE38" s="2" t="s">
+        <v>2345</v>
+      </c>
+      <c r="AF38" s="1">
+        <v>5</v>
       </c>
       <c r="AG38" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AH38" s="10"/>
+        <v>2411</v>
+      </c>
+      <c r="AH38" s="10" t="s">
+        <v>2345</v>
+      </c>
       <c r="AI38" s="1" t="s">
         <v>39</v>
       </c>
@@ -43413,7 +43443,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="39" spans="1:37" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:37" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>128</v>
       </c>
@@ -43526,7 +43556,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="40" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>129</v>
       </c>
@@ -43629,7 +43659,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>129</v>
       </c>
@@ -43732,7 +43762,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>130</v>
       </c>
@@ -43835,7 +43865,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="43" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>133</v>
       </c>
@@ -43938,7 +43968,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="44" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>136</v>
       </c>
@@ -44043,7 +44073,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="45" spans="1:37" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:37" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>146</v>
       </c>
@@ -44152,7 +44182,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="46" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>147</v>
       </c>
@@ -44253,7 +44283,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="47" spans="1:37" ht="60" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:37" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>148</v>
       </c>
@@ -44360,24 +44390,24 @@
         <v>39</v>
       </c>
     </row>
-    <row r="48" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:37" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
-        <v>150</v>
+        <v>123</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>1449</v>
+        <v>157</v>
       </c>
       <c r="C48" s="1">
         <v>2016</v>
       </c>
-      <c r="D48" s="1">
-        <v>12</v>
+      <c r="D48" s="1" t="s">
+        <v>163</v>
       </c>
       <c r="E48" s="1">
-        <v>117</v>
+        <v>13</v>
       </c>
       <c r="F48" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G48" s="1" t="s">
         <v>39</v>
@@ -44387,28 +44417,28 @@
       </c>
       <c r="I48" s="1"/>
       <c r="J48" s="1" t="s">
-        <v>2252</v>
+        <v>2233</v>
       </c>
       <c r="K48" s="1" t="s">
-        <v>605</v>
+        <v>39</v>
       </c>
       <c r="L48" s="1">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="M48" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="N48" s="1" t="s">
-        <v>39</v>
+        <v>654</v>
       </c>
       <c r="O48" s="1" t="s">
-        <v>1839</v>
+        <v>655</v>
       </c>
       <c r="P48" s="1" t="s">
-        <v>687</v>
-      </c>
-      <c r="Q48" s="6">
-        <v>0.91</v>
+        <v>656</v>
+      </c>
+      <c r="Q48" s="1">
+        <v>0.97499999999999998</v>
       </c>
       <c r="R48" s="1" t="s">
         <v>39</v>
@@ -44424,41 +44454,37 @@
         <v>1</v>
       </c>
       <c r="W48" s="1" t="s">
-        <v>2330</v>
+        <v>657</v>
       </c>
       <c r="X48" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y48" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z48" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA48" s="1" t="s">
-        <v>1840</v>
+        <v>0</v>
+      </c>
+      <c r="AA48" s="2" t="s">
+        <v>2383</v>
       </c>
       <c r="AB48" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AC48" s="1">
-        <v>0</v>
+      <c r="AC48" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="AD48" s="1" t="s">
-        <v>1841</v>
-      </c>
-      <c r="AE48" s="2" t="s">
-        <v>2361</v>
-      </c>
-      <c r="AF48" s="1">
-        <v>0</v>
+        <v>39</v>
+      </c>
+      <c r="AE48" s="2"/>
+      <c r="AF48" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="AG48" s="1" t="s">
-        <v>1842</v>
-      </c>
-      <c r="AH48" s="2" t="s">
-        <v>2492</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="AH48" s="10"/>
       <c r="AI48" s="1" t="s">
         <v>39</v>
       </c>
@@ -44469,7 +44495,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="49" spans="1:37" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:37" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>155</v>
       </c>
@@ -44572,7 +44598,7 @@
       <c r="AJ49" s="1"/>
       <c r="AK49" s="1"/>
     </row>
-    <row r="50" spans="1:37" ht="75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:37" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>157</v>
       </c>
@@ -44687,55 +44713,53 @@
     </row>
     <row r="51" spans="1:37" ht="60" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>201</v>
+        <v>1449</v>
       </c>
       <c r="C51" s="1">
-        <v>2015</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>207</v>
+        <v>2016</v>
+      </c>
+      <c r="D51" s="1">
+        <v>12</v>
       </c>
       <c r="E51" s="1">
-        <v>16</v>
+        <v>117</v>
       </c>
       <c r="F51" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>668</v>
+        <v>39</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>669</v>
-      </c>
-      <c r="I51" s="1" t="s">
-        <v>1906</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="I51" s="1"/>
       <c r="J51" s="1" t="s">
-        <v>644</v>
+        <v>2252</v>
       </c>
       <c r="K51" s="1" t="s">
         <v>605</v>
       </c>
       <c r="L51" s="1">
-        <v>3</v>
-      </c>
-      <c r="M51" s="1" t="s">
-        <v>39</v>
+        <v>20</v>
+      </c>
+      <c r="M51" s="1">
+        <v>1</v>
       </c>
       <c r="N51" s="1" t="s">
         <v>39</v>
       </c>
       <c r="O51" s="1" t="s">
-        <v>670</v>
+        <v>1839</v>
       </c>
       <c r="P51" s="1" t="s">
-        <v>671</v>
-      </c>
-      <c r="Q51" s="7">
-        <v>0.79</v>
+        <v>687</v>
+      </c>
+      <c r="Q51" s="6">
+        <v>0.91</v>
       </c>
       <c r="R51" s="1" t="s">
         <v>39</v>
@@ -44751,40 +44775,40 @@
         <v>1</v>
       </c>
       <c r="W51" s="1" t="s">
-        <v>2311</v>
+        <v>2330</v>
       </c>
       <c r="X51" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y51" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z51" s="1">
-        <v>0</v>
-      </c>
-      <c r="AA51" s="1" t="s">
-        <v>2384</v>
+        <v>1</v>
+      </c>
+      <c r="AA51" s="2" t="s">
+        <v>1840</v>
       </c>
       <c r="AB51" s="1" t="s">
         <v>39</v>
       </c>
       <c r="AC51" s="1">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="AD51" s="1" t="s">
-        <v>2385</v>
+        <v>1841</v>
       </c>
       <c r="AE51" s="2" t="s">
-        <v>2699</v>
+        <v>2361</v>
       </c>
       <c r="AF51" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AG51" s="1" t="s">
-        <v>2386</v>
-      </c>
-      <c r="AH51" s="10" t="s">
-        <v>2699</v>
+        <v>1842</v>
+      </c>
+      <c r="AH51" s="2" t="s">
+        <v>2492</v>
       </c>
       <c r="AI51" s="1" t="s">
         <v>39</v>
@@ -44833,8 +44857,8 @@
       <c r="L52" s="1">
         <v>3</v>
       </c>
-      <c r="M52" s="1" t="s">
-        <v>39</v>
+      <c r="M52" s="1">
+        <v>1</v>
       </c>
       <c r="N52" s="1" t="s">
         <v>39</v>
@@ -44869,14 +44893,14 @@
       <c r="X52" s="1">
         <v>0</v>
       </c>
-      <c r="Y52" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z52" s="1" t="s">
-        <v>39</v>
+      <c r="Y52" s="1">
+        <v>2</v>
+      </c>
+      <c r="Z52" s="1">
+        <v>2</v>
       </c>
       <c r="AA52" s="1" t="s">
-        <v>39</v>
+        <v>2793</v>
       </c>
       <c r="AB52" s="1" t="s">
         <v>39</v>
@@ -44909,7 +44933,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="53" spans="1:37" ht="165" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:37" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>166</v>
       </c>
@@ -45022,7 +45046,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="54" spans="1:37" ht="45" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:37" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>173</v>
       </c>
@@ -45131,7 +45155,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="55" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>174</v>
       </c>
@@ -45238,7 +45262,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="56" spans="1:37" ht="60" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:37" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>178</v>
       </c>
@@ -45343,7 +45367,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="57" spans="1:37" ht="45" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:37" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>180</v>
       </c>
@@ -45456,7 +45480,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="58" spans="1:37" ht="45" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:37" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>180</v>
       </c>
@@ -45569,7 +45593,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="59" spans="1:37" ht="45" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:37" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>180</v>
       </c>
@@ -45680,21 +45704,21 @@
         <v>39</v>
       </c>
     </row>
-    <row r="60" spans="1:37" ht="60" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:37" ht="135" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
-        <v>183</v>
+        <v>111</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>910</v>
+        <v>148</v>
       </c>
       <c r="C60" s="1">
-        <v>2020</v>
-      </c>
-      <c r="D60" s="1">
-        <v>17</v>
-      </c>
-      <c r="E60" s="1">
-        <v>69</v>
+        <v>2010</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>877</v>
       </c>
       <c r="F60" s="1">
         <v>0</v>
@@ -45706,72 +45730,82 @@
         <v>39</v>
       </c>
       <c r="I60" s="1"/>
-      <c r="J60" s="1"/>
+      <c r="J60" s="1" t="s">
+        <v>650</v>
+      </c>
       <c r="K60" s="1" t="s">
         <v>605</v>
       </c>
       <c r="L60" s="1">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="M60" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="N60" s="1" t="s">
-        <v>2268</v>
+        <v>39</v>
       </c>
       <c r="O60" s="1" t="s">
-        <v>2296</v>
+        <v>651</v>
       </c>
       <c r="P60" s="1" t="s">
-        <v>1276</v>
-      </c>
-      <c r="Q60" s="6">
-        <v>0.86</v>
-      </c>
+        <v>652</v>
+      </c>
+      <c r="Q60" s="6"/>
       <c r="R60" s="1" t="s">
-        <v>1277</v>
+        <v>653</v>
       </c>
       <c r="S60" s="1">
-        <v>0.84499999999999997</v>
-      </c>
-      <c r="T60" s="1"/>
+        <v>0.98199999999999998</v>
+      </c>
+      <c r="T60" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="U60" s="1" t="s">
         <v>39</v>
       </c>
       <c r="V60" s="1">
-        <v>0</v>
-      </c>
-      <c r="W60" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="X60" s="1"/>
-      <c r="Y60" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z60" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AA60" s="1" t="s">
-        <v>39</v>
+        <v>1</v>
+      </c>
+      <c r="W60" s="12" t="s">
+        <v>2310</v>
+      </c>
+      <c r="X60" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y60" s="1">
+        <v>2</v>
+      </c>
+      <c r="Z60" s="1">
+        <v>2</v>
+      </c>
+      <c r="AA60" s="2" t="s">
+        <v>2341</v>
       </c>
       <c r="AB60" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AC60" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AD60" s="1"/>
-      <c r="AE60" s="2"/>
+      <c r="AC60" s="1">
+        <v>5</v>
+      </c>
+      <c r="AD60" s="1" t="s">
+        <v>2501</v>
+      </c>
+      <c r="AE60" s="2" t="s">
+        <v>2723</v>
+      </c>
       <c r="AF60" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="AG60" s="1" t="s">
-        <v>2418</v>
+        <v>2502</v>
       </c>
       <c r="AH60" s="10" t="s">
-        <v>2757</v>
-      </c>
-      <c r="AI60" s="1"/>
+        <v>2723</v>
+      </c>
+      <c r="AI60" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="AJ60" s="1" t="s">
         <v>39</v>
       </c>
@@ -45779,7 +45813,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="61" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>188</v>
       </c>
@@ -45880,7 +45914,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="62" spans="1:37" ht="60" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:37" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>193</v>
       </c>
@@ -45991,7 +46025,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="63" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>200</v>
       </c>
@@ -46098,7 +46132,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="64" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>201</v>
       </c>
@@ -46199,7 +46233,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="65" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>210</v>
       </c>
@@ -46300,7 +46334,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="66" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>214</v>
       </c>
@@ -46403,7 +46437,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="67" spans="1:37" ht="30" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:37" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>216</v>
       </c>
@@ -46512,7 +46546,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="68" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>219</v>
       </c>
@@ -46617,7 +46651,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="69" spans="1:37" ht="45" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:37" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>220</v>
       </c>
@@ -46728,7 +46762,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="70" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>233</v>
       </c>
@@ -46829,7 +46863,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="71" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>234</v>
       </c>
@@ -46932,7 +46966,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="72" spans="1:37" ht="60" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:37" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>236</v>
       </c>
@@ -47039,7 +47073,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="73" spans="1:37" ht="60" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:37" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>242</v>
       </c>
@@ -47146,7 +47180,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="74" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>248</v>
       </c>
@@ -47245,7 +47279,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="75" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>253</v>
       </c>
@@ -47344,7 +47378,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="76" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>254</v>
       </c>
@@ -47445,7 +47479,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="77" spans="1:37" ht="30" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:37" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>262</v>
       </c>
@@ -47554,7 +47588,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="78" spans="1:37" ht="60" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:37" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>263</v>
       </c>
@@ -47665,7 +47699,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="79" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>269</v>
       </c>
@@ -47766,7 +47800,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="80" spans="1:37" ht="45" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:37" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>270</v>
       </c>
@@ -47877,7 +47911,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="81" spans="1:37" ht="75" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:37" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>274</v>
       </c>
@@ -47984,7 +48018,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="82" spans="1:37" ht="45" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:37" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>279</v>
       </c>
@@ -48087,7 +48121,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="83" spans="1:37" ht="45" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:37" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>280</v>
       </c>
@@ -48194,7 +48228,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="84" spans="1:37" ht="90" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:37" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>291</v>
       </c>
@@ -48305,7 +48339,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="85" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>301</v>
       </c>
@@ -48406,7 +48440,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="86" spans="1:37" ht="45" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:37" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>302</v>
       </c>
@@ -48517,7 +48551,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="87" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>303</v>
       </c>
@@ -48620,7 +48654,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="88" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>312</v>
       </c>
@@ -48723,7 +48757,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="89" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>324</v>
       </c>
@@ -48828,7 +48862,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="90" spans="1:37" ht="135" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:37" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>325</v>
       </c>
@@ -48937,7 +48971,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="91" spans="1:37" ht="60" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:37" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>327</v>
       </c>
@@ -49040,7 +49074,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="92" spans="1:37" ht="45" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:37" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>335</v>
       </c>
@@ -49149,7 +49183,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="93" spans="1:37" ht="75" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:37" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>337</v>
       </c>
@@ -49287,8 +49321,8 @@
       <c r="L94" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="M94" s="1" t="s">
-        <v>39</v>
+      <c r="M94" s="1">
+        <v>1</v>
       </c>
       <c r="N94" s="1" t="s">
         <v>39</v>
@@ -49327,7 +49361,7 @@
       <c r="Z94" s="1">
         <v>2</v>
       </c>
-      <c r="AA94" s="1" t="s">
+      <c r="AA94" s="2" t="s">
         <v>1887</v>
       </c>
       <c r="AB94" s="1"/>
@@ -49359,7 +49393,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="95" spans="1:37" ht="60" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:37" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>339</v>
       </c>
@@ -49466,7 +49500,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="96" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>342</v>
       </c>
@@ -49573,7 +49607,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="97" spans="1:37" ht="60" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:37" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>346</v>
       </c>
@@ -49686,7 +49720,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="98" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>347</v>
       </c>
@@ -49779,7 +49813,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="99" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>348</v>
       </c>
@@ -49884,7 +49918,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="100" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:37" ht="105" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>349</v>
       </c>
@@ -49961,7 +49995,7 @@
       <c r="Z100" s="1">
         <v>2</v>
       </c>
-      <c r="AA100" s="1" t="s">
+      <c r="AA100" s="2" t="s">
         <v>1896</v>
       </c>
       <c r="AB100" s="1" t="s">
@@ -49993,7 +50027,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="101" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>352</v>
       </c>
@@ -50098,7 +50132,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="102" spans="1:37" ht="45" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:37" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>355</v>
       </c>
@@ -50207,7 +50241,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="103" spans="1:37" ht="90" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:37" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>362</v>
       </c>
@@ -50312,7 +50346,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="104" spans="1:37" ht="45" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:37" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>363</v>
       </c>
@@ -50421,7 +50455,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="105" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>367</v>
       </c>
@@ -50528,7 +50562,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="106" spans="1:37" ht="45" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:37" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>371</v>
       </c>
@@ -50637,7 +50671,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="107" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>372</v>
       </c>
@@ -50736,7 +50770,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="108" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>372</v>
       </c>
@@ -50835,7 +50869,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="109" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>372</v>
       </c>
@@ -50938,7 +50972,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="110" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>376</v>
       </c>
@@ -51043,7 +51077,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="111" spans="1:37" ht="90" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:37" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>378</v>
       </c>
@@ -51154,61 +51188,63 @@
         <v>39</v>
       </c>
     </row>
-    <row r="112" spans="1:37" ht="30" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:37" ht="180" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
-        <v>381</v>
+        <v>675</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>1606</v>
+        <v>549</v>
       </c>
       <c r="C112" s="1">
-        <v>2016</v>
+        <v>2020</v>
       </c>
       <c r="D112" s="1">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E112" s="1">
-        <v>135</v>
+        <v>101</v>
       </c>
       <c r="F112" s="1">
         <v>1</v>
       </c>
       <c r="G112" s="1" t="s">
-        <v>1905</v>
+        <v>672</v>
       </c>
       <c r="H112" s="1" t="s">
-        <v>1906</v>
+        <v>2263</v>
       </c>
       <c r="I112" s="1" t="s">
-        <v>1906</v>
+        <v>703</v>
       </c>
       <c r="J112" s="1" t="s">
-        <v>731</v>
+        <v>2250</v>
       </c>
       <c r="K112" s="1" t="s">
-        <v>39</v>
+        <v>767</v>
       </c>
       <c r="L112" s="1">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="M112" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N112" s="1" t="s">
-        <v>1907</v>
+        <v>39</v>
       </c>
       <c r="O112" s="1" t="s">
-        <v>2292</v>
+        <v>1361</v>
       </c>
       <c r="P112" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q112" s="6"/>
+        <v>666</v>
+      </c>
+      <c r="Q112" s="6">
+        <v>0.89</v>
+      </c>
       <c r="R112" s="1" t="s">
-        <v>1908</v>
+        <v>661</v>
       </c>
       <c r="S112" s="1">
-        <v>0.69899999999999995</v>
+        <v>0.93</v>
       </c>
       <c r="T112" s="1" t="s">
         <v>39</v>
@@ -51217,39 +51253,45 @@
         <v>39</v>
       </c>
       <c r="V112" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W112" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="X112" s="1"/>
-      <c r="Y112" s="1"/>
-      <c r="Z112" s="1"/>
-      <c r="AA112" s="1"/>
+        <v>1362</v>
+      </c>
+      <c r="X112" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y112" s="1" t="s">
+        <v>2336</v>
+      </c>
+      <c r="Z112" s="1">
+        <v>4</v>
+      </c>
+      <c r="AA112" s="2" t="s">
+        <v>2440</v>
+      </c>
       <c r="AB112" s="1" t="s">
-        <v>39</v>
+        <v>2340</v>
       </c>
       <c r="AC112" s="1">
         <v>5</v>
       </c>
       <c r="AD112" s="1" t="s">
-        <v>2459</v>
+        <v>2441</v>
       </c>
       <c r="AE112" s="2" t="s">
-        <v>2751</v>
+        <v>2062</v>
       </c>
       <c r="AF112" s="1">
         <v>5</v>
       </c>
       <c r="AG112" s="1" t="s">
-        <v>2460</v>
+        <v>2442</v>
       </c>
       <c r="AH112" s="2" t="s">
-        <v>2751</v>
-      </c>
-      <c r="AI112" s="1" t="s">
-        <v>39</v>
-      </c>
+        <v>2062</v>
+      </c>
+      <c r="AI112" s="1"/>
       <c r="AJ112" s="1" t="s">
         <v>39</v>
       </c>
@@ -51257,7 +51299,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="113" spans="1:37" ht="75" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:37" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>384</v>
       </c>
@@ -51368,7 +51410,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="114" spans="1:37" ht="120" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:37" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>400</v>
       </c>
@@ -51477,7 +51519,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="115" spans="1:37" ht="30" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:37" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>405</v>
       </c>
@@ -51584,7 +51626,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="116" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>408</v>
       </c>
@@ -51691,7 +51733,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="117" spans="1:37" ht="75" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:37" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>412</v>
       </c>
@@ -51800,7 +51842,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="118" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>418</v>
       </c>
@@ -51899,7 +51941,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="119" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>419</v>
       </c>
@@ -52004,7 +52046,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="120" spans="1:37" ht="45" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:37" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>429</v>
       </c>
@@ -52111,7 +52153,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="121" spans="1:37" ht="45" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:37" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>430</v>
       </c>
@@ -52214,7 +52256,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="122" spans="1:37" ht="60" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:37" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>433</v>
       </c>
@@ -52321,7 +52363,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="123" spans="1:37" ht="60" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:37" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>438</v>
       </c>
@@ -52432,7 +52474,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="124" spans="1:37" ht="60" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:37" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>441</v>
       </c>
@@ -52509,7 +52551,7 @@
       <c r="AJ124" s="1"/>
       <c r="AK124" s="1"/>
     </row>
-    <row r="125" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>442</v>
       </c>
@@ -52614,7 +52656,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="126" spans="1:37" ht="60" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:37" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>452</v>
       </c>
@@ -52721,7 +52763,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="127" spans="1:37" ht="45" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:37" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>465</v>
       </c>
@@ -52826,7 +52868,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="128" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>479</v>
       </c>
@@ -52929,7 +52971,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="129" spans="1:37" ht="90" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:37" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>482</v>
       </c>
@@ -53028,7 +53070,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="130" spans="1:37" ht="165" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:37" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>486</v>
       </c>
@@ -53131,7 +53173,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="131" spans="1:37" ht="225" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:37" ht="225" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>497</v>
       </c>
@@ -53238,7 +53280,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="132" spans="1:37" ht="30" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:37" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>498</v>
       </c>
@@ -53349,62 +53391,62 @@
         <v>39</v>
       </c>
     </row>
-    <row r="133" spans="1:37" ht="30" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:37" ht="135" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
-        <v>501</v>
+        <v>81</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>1093</v>
+        <v>1413</v>
       </c>
       <c r="C133" s="1">
-        <v>2020</v>
+        <v>2016</v>
       </c>
       <c r="D133" s="1">
-        <v>39</v>
-      </c>
-      <c r="E133" s="1" t="s">
-        <v>2198</v>
-      </c>
-      <c r="F133" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="E133" s="1">
+        <v>112</v>
+      </c>
+      <c r="F133" s="1">
+        <v>1</v>
+      </c>
       <c r="G133" s="1" t="s">
-        <v>1331</v>
+        <v>1827</v>
       </c>
       <c r="H133" s="1" t="s">
-        <v>626</v>
+        <v>1828</v>
       </c>
       <c r="I133" s="1" t="s">
-        <v>626</v>
+        <v>2229</v>
       </c>
       <c r="J133" s="1" t="s">
-        <v>731</v>
+        <v>2251</v>
       </c>
       <c r="K133" s="1" t="s">
-        <v>605</v>
+        <v>727</v>
       </c>
       <c r="L133" s="1">
-        <v>2</v>
-      </c>
-      <c r="M133" s="1" t="s">
-        <v>39</v>
+        <v>4</v>
+      </c>
+      <c r="M133" s="1">
+        <v>1</v>
       </c>
       <c r="N133" s="1" t="s">
-        <v>39</v>
+        <v>1829</v>
       </c>
       <c r="O133" s="1" t="s">
-        <v>2285</v>
+        <v>1830</v>
       </c>
       <c r="P133" s="1" t="s">
-        <v>1097</v>
+        <v>1831</v>
       </c>
       <c r="Q133" s="6">
-        <v>0.79</v>
+        <v>0.73</v>
       </c>
       <c r="R133" s="1" t="s">
-        <v>1097</v>
-      </c>
-      <c r="S133" s="1">
-        <v>0.79</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="S133" s="1"/>
       <c r="T133" s="1" t="s">
         <v>39</v>
       </c>
@@ -53412,41 +53454,43 @@
         <v>39</v>
       </c>
       <c r="V133" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W133" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="X133" s="1"/>
+        <v>1832</v>
+      </c>
+      <c r="X133" s="1">
+        <v>0</v>
+      </c>
       <c r="Y133" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z133" s="1">
-        <v>0</v>
-      </c>
-      <c r="AA133" s="1" t="s">
-        <v>1332</v>
+        <v>1</v>
+      </c>
+      <c r="AA133" s="2" t="s">
+        <v>2795</v>
       </c>
       <c r="AB133" s="1" t="s">
-        <v>39</v>
+        <v>2794</v>
       </c>
       <c r="AC133" s="1">
         <v>5</v>
       </c>
       <c r="AD133" s="1" t="s">
-        <v>1333</v>
+        <v>2447</v>
       </c>
       <c r="AE133" s="2" t="s">
-        <v>2357</v>
-      </c>
-      <c r="AF133" s="1" t="s">
-        <v>39</v>
+        <v>2746</v>
+      </c>
+      <c r="AF133" s="1">
+        <v>5</v>
       </c>
       <c r="AG133" s="1" t="s">
-        <v>39</v>
+        <v>2447</v>
       </c>
       <c r="AH133" s="2" t="s">
-        <v>39</v>
+        <v>2746</v>
       </c>
       <c r="AI133" s="1" t="s">
         <v>39</v>
@@ -53458,7 +53502,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="134" spans="1:37" ht="75" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:37" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>517</v>
       </c>
@@ -53571,7 +53615,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="135" spans="1:37" ht="45" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:37" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>523</v>
       </c>
@@ -53682,7 +53726,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="136" spans="1:37" ht="30" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:37" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>524</v>
       </c>
@@ -53787,7 +53831,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="137" spans="1:37" ht="90" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:37" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>528</v>
       </c>
@@ -53896,7 +53940,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="138" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>531</v>
       </c>
@@ -54001,7 +54045,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="139" spans="1:37" ht="30" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:37" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>533</v>
       </c>
@@ -54110,7 +54154,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="140" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>536</v>
       </c>
@@ -54207,112 +54251,94 @@
         <v>39</v>
       </c>
     </row>
-    <row r="141" spans="1:37" ht="30" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:37" ht="60" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
-        <v>540</v>
+        <v>183</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>492</v>
+        <v>910</v>
       </c>
       <c r="C141" s="1">
-        <v>2018</v>
-      </c>
-      <c r="D141" s="1" t="s">
-        <v>497</v>
-      </c>
-      <c r="E141" s="1" t="s">
-        <v>2183</v>
+        <v>2020</v>
+      </c>
+      <c r="D141" s="1">
+        <v>17</v>
+      </c>
+      <c r="E141" s="1">
+        <v>69</v>
       </c>
       <c r="F141" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G141" s="1" t="s">
-        <v>751</v>
+        <v>39</v>
       </c>
       <c r="H141" s="1" t="s">
-        <v>752</v>
-      </c>
-      <c r="I141" s="1" t="s">
-        <v>703</v>
-      </c>
-      <c r="J141" s="1" t="s">
-        <v>731</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="I141" s="1"/>
+      <c r="J141" s="1"/>
       <c r="K141" s="1" t="s">
-        <v>753</v>
+        <v>605</v>
       </c>
       <c r="L141" s="1">
-        <v>3</v>
-      </c>
-      <c r="M141" s="1" t="s">
-        <v>39</v>
+        <v>20</v>
+      </c>
+      <c r="M141" s="1">
+        <v>4</v>
       </c>
       <c r="N141" s="1" t="s">
-        <v>39</v>
+        <v>2268</v>
       </c>
       <c r="O141" s="1" t="s">
-        <v>754</v>
+        <v>2296</v>
       </c>
       <c r="P141" s="1" t="s">
-        <v>755</v>
-      </c>
-      <c r="Q141" s="1">
-        <v>0.85</v>
+        <v>1276</v>
+      </c>
+      <c r="Q141" s="6">
+        <v>0.86</v>
       </c>
       <c r="R141" s="1" t="s">
-        <v>756</v>
+        <v>1277</v>
       </c>
       <c r="S141" s="1">
-        <v>0.86</v>
-      </c>
-      <c r="T141" s="1" t="s">
-        <v>39</v>
-      </c>
+        <v>0.84499999999999997</v>
+      </c>
+      <c r="T141" s="1"/>
       <c r="U141" s="1" t="s">
         <v>39</v>
       </c>
       <c r="V141" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W141" s="1" t="s">
-        <v>2319</v>
-      </c>
-      <c r="X141" s="1">
-        <v>0</v>
-      </c>
-      <c r="Y141" s="1">
-        <v>0</v>
-      </c>
-      <c r="Z141" s="1">
-        <v>0</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="X141" s="1"/>
+      <c r="Y141" s="1"/>
+      <c r="Z141" s="1"/>
       <c r="AA141" s="1" t="s">
-        <v>2409</v>
+        <v>2797</v>
       </c>
       <c r="AB141" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AC141" s="1">
-        <v>5</v>
-      </c>
-      <c r="AD141" s="1" t="s">
-        <v>2410</v>
-      </c>
-      <c r="AE141" s="2" t="s">
-        <v>2345</v>
-      </c>
+      <c r="AC141" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD141" s="1"/>
+      <c r="AE141" s="2"/>
       <c r="AF141" s="1">
         <v>5</v>
       </c>
       <c r="AG141" s="1" t="s">
-        <v>2411</v>
+        <v>2418</v>
       </c>
       <c r="AH141" s="10" t="s">
-        <v>2345</v>
-      </c>
-      <c r="AI141" s="1" t="s">
-        <v>39</v>
-      </c>
+        <v>2757</v>
+      </c>
+      <c r="AI141" s="1"/>
       <c r="AJ141" s="1" t="s">
         <v>39</v>
       </c>
@@ -54320,7 +54346,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="142" spans="1:37" ht="45" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:37" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>545</v>
       </c>
@@ -54425,7 +54451,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="143" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>550</v>
       </c>
@@ -54530,7 +54556,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="144" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <v>553</v>
       </c>
@@ -54633,7 +54659,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="145" spans="1:37" ht="60" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:37" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>557</v>
       </c>
@@ -54740,7 +54766,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="146" spans="1:37" ht="60" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:37" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>558</v>
       </c>
@@ -54849,7 +54875,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="147" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>560</v>
       </c>
@@ -54954,7 +54980,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="148" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>561</v>
       </c>
@@ -55061,7 +55087,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="149" spans="1:37" ht="45" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:37" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>569</v>
       </c>
@@ -55168,7 +55194,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="150" spans="1:37" ht="75" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:37" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>573</v>
       </c>
@@ -55275,7 +55301,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="151" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <v>574</v>
       </c>
@@ -55380,7 +55406,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="152" spans="1:37" ht="60" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:37" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>590</v>
       </c>
@@ -55489,7 +55515,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="153" spans="1:37" ht="45" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:37" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
         <v>600</v>
       </c>
@@ -55592,7 +55618,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="154" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <v>626</v>
       </c>
@@ -55697,7 +55723,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="155" spans="1:37" ht="45" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:37" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
         <v>627</v>
       </c>
@@ -55806,7 +55832,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="156" spans="1:37" ht="45" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:37" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <v>628</v>
       </c>
@@ -55917,7 +55943,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="157" spans="1:37" ht="90" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:37" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
         <v>636</v>
       </c>
@@ -56022,7 +56048,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="158" spans="1:37" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:37" s="3" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
         <v>640</v>
       </c>
@@ -56131,7 +56157,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="159" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
         <v>650</v>
       </c>
@@ -56230,7 +56256,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="160" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
         <v>659</v>
       </c>
@@ -56329,7 +56355,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="161" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
         <v>660</v>
       </c>
@@ -56434,7 +56460,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="162" spans="1:37" ht="60" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:37" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
         <v>672</v>
       </c>
@@ -56543,63 +56569,61 @@
         <v>39</v>
       </c>
     </row>
-    <row r="163" spans="1:37" ht="45" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:37" ht="90" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
-        <v>675</v>
+        <v>381</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>549</v>
+        <v>1606</v>
       </c>
       <c r="C163" s="1">
-        <v>2020</v>
+        <v>2016</v>
       </c>
       <c r="D163" s="1">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="E163" s="1">
-        <v>101</v>
+        <v>135</v>
       </c>
       <c r="F163" s="1">
         <v>1</v>
       </c>
       <c r="G163" s="1" t="s">
-        <v>672</v>
+        <v>1905</v>
       </c>
       <c r="H163" s="1" t="s">
-        <v>2263</v>
+        <v>1906</v>
       </c>
       <c r="I163" s="1" t="s">
-        <v>703</v>
+        <v>1906</v>
       </c>
       <c r="J163" s="1" t="s">
-        <v>2250</v>
+        <v>731</v>
       </c>
       <c r="K163" s="1" t="s">
-        <v>767</v>
+        <v>39</v>
       </c>
       <c r="L163" s="1">
-        <v>3</v>
-      </c>
-      <c r="M163" s="1" t="s">
-        <v>39</v>
+        <v>8</v>
+      </c>
+      <c r="M163" s="1">
+        <v>2</v>
       </c>
       <c r="N163" s="1" t="s">
-        <v>39</v>
+        <v>1907</v>
       </c>
       <c r="O163" s="1" t="s">
-        <v>1361</v>
+        <v>2292</v>
       </c>
       <c r="P163" s="1" t="s">
-        <v>666</v>
-      </c>
-      <c r="Q163" s="6">
-        <v>0.89</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="Q163" s="6"/>
       <c r="R163" s="1" t="s">
-        <v>661</v>
+        <v>1908</v>
       </c>
       <c r="S163" s="1">
-        <v>0.93</v>
+        <v>0.69899999999999995</v>
       </c>
       <c r="T163" s="1" t="s">
         <v>39</v>
@@ -56608,45 +56632,45 @@
         <v>39</v>
       </c>
       <c r="V163" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W163" s="1" t="s">
-        <v>1362</v>
-      </c>
-      <c r="X163" s="1">
-        <v>1</v>
-      </c>
-      <c r="Y163" s="1" t="s">
-        <v>2336</v>
+        <v>39</v>
+      </c>
+      <c r="X163" s="1"/>
+      <c r="Y163" s="1">
+        <v>0</v>
       </c>
       <c r="Z163" s="1">
-        <v>4</v>
-      </c>
-      <c r="AA163" s="1" t="s">
-        <v>2440</v>
+        <v>0</v>
+      </c>
+      <c r="AA163" s="2" t="s">
+        <v>2796</v>
       </c>
       <c r="AB163" s="1" t="s">
-        <v>2340</v>
+        <v>39</v>
       </c>
       <c r="AC163" s="1">
         <v>5</v>
       </c>
       <c r="AD163" s="1" t="s">
-        <v>2441</v>
+        <v>2459</v>
       </c>
       <c r="AE163" s="2" t="s">
-        <v>2062</v>
+        <v>2751</v>
       </c>
       <c r="AF163" s="1">
         <v>5</v>
       </c>
       <c r="AG163" s="1" t="s">
-        <v>2442</v>
+        <v>2460</v>
       </c>
       <c r="AH163" s="2" t="s">
-        <v>2062</v>
-      </c>
-      <c r="AI163" s="1"/>
+        <v>2751</v>
+      </c>
+      <c r="AI163" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="AJ163" s="1" t="s">
         <v>39</v>
       </c>
@@ -56654,7 +56678,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="164" spans="1:37" ht="90" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:37" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
         <v>676</v>
       </c>
@@ -56765,7 +56789,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="165" spans="1:37" ht="75" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:37" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
         <v>677</v>
       </c>
@@ -56862,7 +56886,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="166" spans="1:37" ht="75" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:37" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <v>678</v>
       </c>
@@ -56971,7 +56995,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="167" spans="1:37" ht="60" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:37" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
         <v>682</v>
       </c>
@@ -57078,7 +57102,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="168" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
         <v>684</v>
       </c>
@@ -57185,7 +57209,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="169" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
         <v>685</v>
       </c>
@@ -57294,7 +57318,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="170" spans="1:37" ht="45" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:37" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
         <v>686</v>
       </c>
@@ -57399,7 +57423,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="171" spans="1:37" ht="75" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:37" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
         <v>687</v>
       </c>
@@ -57506,7 +57530,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="172" spans="1:37" ht="30" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:37" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
         <v>688</v>
       </c>
@@ -57617,7 +57641,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="173" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:37" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
         <v>689</v>
       </c>
@@ -57724,7 +57748,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="174" spans="1:37" ht="30" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:37" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
         <v>690</v>
       </c>

</xml_diff>

<commit_message>
added analysis on double reliability reported
</commit_message>
<xml_diff>
--- a/data/raw/Review_data_all_packages.xlsx
+++ b/data/raw/Review_data_all_packages.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neleb\Documents\GitHub\CSE-review\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6306F8B-B6F2-4F05-947F-BA5B1115102A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FB8B099-275A-4962-8684-BC18075E7834}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="15585" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9832" uniqueCount="2798">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9831" uniqueCount="2797">
   <si>
     <t>id</t>
   </si>
@@ -8957,9 +8957,6 @@
   </si>
   <si>
     <t>Exploratory factor analyses were used to assess convergent and discriminant validity: All eigenvalues associated with the factors exceeded the required level of 1.0, varying from 1.14 to 3.73; As shown in Table 1, the overall factor structural solution had an appropriate loading pattern and explained 68.94 percent of the variation.</t>
-  </si>
-  <si>
-    <t>no specific reporting</t>
   </si>
 </sst>
 </file>
@@ -9036,7 +9033,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -9059,7 +9056,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -10803,7 +10799,13 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B8C8C23E-B8AC-4554-A9ED-C1B262734E5B}" name="Tabelle1" displayName="Tabelle1" ref="A1:BC185" totalsRowShown="0" headerRowDxfId="100" dataDxfId="99">
-  <autoFilter ref="A1:BC185" xr:uid="{B8C8C23E-B8AC-4554-A9ED-C1B262734E5B}"/>
+  <autoFilter ref="A1:BC185" xr:uid="{B8C8C23E-B8AC-4554-A9ED-C1B262734E5B}">
+    <filterColumn colId="28">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:BC185">
     <sortCondition ref="A1:A185"/>
   </sortState>
@@ -11232,8 +11234,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BC185"/>
   <sheetViews>
-    <sheetView topLeftCell="U1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AB11" sqref="AB11"/>
+    <sheetView topLeftCell="W1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AC53" activeCellId="2" sqref="AC1:AC1048576 AC13 AC53 AC56 AC66 AC69 AC137 AC141 AC160 AC186:AC1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11457,7 +11459,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -11601,7 +11603,7 @@
         <v>779</v>
       </c>
     </row>
-    <row r="3" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>4</v>
       </c>
@@ -11756,7 +11758,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>8</v>
       </c>
@@ -11911,7 +11913,7 @@
         <v>2181</v>
       </c>
     </row>
-    <row r="5" spans="1:55" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:55" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>10</v>
       </c>
@@ -12072,7 +12074,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:55" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:55" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>11</v>
       </c>
@@ -12233,7 +12235,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>15</v>
       </c>
@@ -12388,7 +12390,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>19</v>
       </c>
@@ -12543,7 +12545,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="9" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>25</v>
       </c>
@@ -12698,7 +12700,7 @@
         <v>779</v>
       </c>
     </row>
-    <row r="10" spans="1:55" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:55" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>26</v>
       </c>
@@ -12853,7 +12855,7 @@
         <v>2179</v>
       </c>
     </row>
-    <row r="11" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>28</v>
       </c>
@@ -13008,7 +13010,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>32</v>
       </c>
@@ -13312,7 +13314,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>36</v>
       </c>
@@ -13459,7 +13461,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:55" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:55" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>42</v>
       </c>
@@ -13614,7 +13616,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>43</v>
       </c>
@@ -13754,7 +13756,7 @@
         <v>2179</v>
       </c>
     </row>
-    <row r="17" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>43</v>
       </c>
@@ -13912,7 +13914,7 @@
         <v>2179</v>
       </c>
     </row>
-    <row r="18" spans="1:55" ht="120" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:55" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>56</v>
       </c>
@@ -14065,7 +14067,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>56</v>
       </c>
@@ -14202,7 +14204,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>56</v>
       </c>
@@ -14339,7 +14341,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>56</v>
       </c>
@@ -14476,7 +14478,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>61</v>
       </c>
@@ -14631,7 +14633,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>62</v>
       </c>
@@ -14780,7 +14782,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="24" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>79</v>
       </c>
@@ -14935,7 +14937,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>81</v>
       </c>
@@ -15090,7 +15092,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="26" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>82</v>
       </c>
@@ -15226,7 +15228,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>83</v>
       </c>
@@ -15376,7 +15378,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="1:55" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:55" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>86</v>
       </c>
@@ -15531,7 +15533,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="29" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>87</v>
       </c>
@@ -15683,7 +15685,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="30" spans="1:55" ht="105" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:55" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>94</v>
       </c>
@@ -15827,7 +15829,7 @@
         <v>2179</v>
       </c>
     </row>
-    <row r="31" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>94</v>
       </c>
@@ -15971,7 +15973,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="32" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>94</v>
       </c>
@@ -16115,7 +16117,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="33" spans="1:55" ht="45" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:55" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>95</v>
       </c>
@@ -16262,7 +16264,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="34" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>98</v>
       </c>
@@ -16417,7 +16419,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="35" spans="1:55" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:55" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>99</v>
       </c>
@@ -16575,7 +16577,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="36" spans="1:55" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:55" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>111</v>
       </c>
@@ -16730,7 +16732,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="37" spans="1:55" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:55" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>116</v>
       </c>
@@ -16882,7 +16884,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>123</v>
       </c>
@@ -17037,7 +17039,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="39" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>124</v>
       </c>
@@ -17195,7 +17197,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="40" spans="1:55" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:55" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>128</v>
       </c>
@@ -17350,7 +17352,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="41" spans="1:55" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:55" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>129</v>
       </c>
@@ -17492,7 +17494,7 @@
         <v>878</v>
       </c>
     </row>
-    <row r="42" spans="1:55" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:55" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>129</v>
       </c>
@@ -17634,7 +17636,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="43" spans="1:55" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:55" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>130</v>
       </c>
@@ -17787,7 +17789,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="44" spans="1:55" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:55" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>133</v>
       </c>
@@ -17948,7 +17950,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="45" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>136</v>
       </c>
@@ -18103,7 +18105,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="46" spans="1:55" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:55" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>146</v>
       </c>
@@ -18258,7 +18260,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="47" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>147</v>
       </c>
@@ -18410,7 +18412,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="48" spans="1:55" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:55" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>148</v>
       </c>
@@ -18557,7 +18559,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="49" spans="1:55" ht="150" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:55" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>150</v>
       </c>
@@ -18709,7 +18711,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="50" spans="1:55" ht="45" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:55" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>155</v>
       </c>
@@ -18858,7 +18860,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="51" spans="1:55" ht="120" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:55" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>157</v>
       </c>
@@ -19013,7 +19015,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="52" spans="1:55" ht="30" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:55" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>162</v>
       </c>
@@ -19326,7 +19328,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="54" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>166</v>
       </c>
@@ -19472,7 +19474,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="55" spans="1:55" ht="30" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:55" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>173</v>
       </c>
@@ -19788,7 +19790,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="57" spans="1:55" ht="90" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:55" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>178</v>
       </c>
@@ -19935,7 +19937,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="58" spans="1:55" ht="30" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:55" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>180</v>
       </c>
@@ -20090,7 +20092,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="59" spans="1:55" ht="30" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:55" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>180</v>
       </c>
@@ -20245,7 +20247,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="60" spans="1:55" ht="30" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:55" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>180</v>
       </c>
@@ -20400,7 +20402,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="61" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>183</v>
       </c>
@@ -20547,7 +20549,7 @@
         <v>917</v>
       </c>
     </row>
-    <row r="62" spans="1:55" ht="30" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:55" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>188</v>
       </c>
@@ -20693,7 +20695,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="1:55" ht="30" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:55" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>193</v>
       </c>
@@ -20848,7 +20850,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="64" spans="1:55" ht="60" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:55" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>200</v>
       </c>
@@ -21003,7 +21005,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="65" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>201</v>
       </c>
@@ -21307,7 +21309,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="67" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>214</v>
       </c>
@@ -21462,7 +21464,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="68" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>216</v>
       </c>
@@ -21764,7 +21766,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="70" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>220</v>
       </c>
@@ -21905,7 +21907,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="71" spans="1:55" ht="30" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:55" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>233</v>
       </c>
@@ -22060,7 +22062,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="72" spans="1:55" ht="90" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:55" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>234</v>
       </c>
@@ -22216,7 +22218,7 @@
         <v>2178</v>
       </c>
     </row>
-    <row r="73" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>236</v>
       </c>
@@ -22374,7 +22376,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="74" spans="1:55" ht="30" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:55" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>242</v>
       </c>
@@ -22530,7 +22532,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="75" spans="1:55" ht="60" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:55" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>248</v>
       </c>
@@ -22685,7 +22687,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="76" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>253</v>
       </c>
@@ -22840,7 +22842,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="77" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>254</v>
       </c>
@@ -22995,7 +22997,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="78" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>262</v>
       </c>
@@ -23150,7 +23152,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="79" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>263</v>
       </c>
@@ -23297,7 +23299,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="80" spans="1:55" ht="30" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:55" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>269</v>
       </c>
@@ -23441,7 +23443,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="81" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>270</v>
       </c>
@@ -23596,7 +23598,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="82" spans="1:55" ht="30" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:55" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>274</v>
       </c>
@@ -23751,7 +23753,7 @@
         <v>982</v>
       </c>
     </row>
-    <row r="83" spans="1:55" ht="30" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:55" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>279</v>
       </c>
@@ -23903,7 +23905,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="84" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>280</v>
       </c>
@@ -24056,7 +24058,7 @@
         <v>917</v>
       </c>
     </row>
-    <row r="85" spans="1:55" ht="30" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:55" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>291</v>
       </c>
@@ -24211,7 +24213,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="86" spans="1:55" ht="60" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:55" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>301</v>
       </c>
@@ -24359,7 +24361,7 @@
         <v>2179</v>
       </c>
     </row>
-    <row r="87" spans="1:55" ht="30" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:55" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>302</v>
       </c>
@@ -24514,7 +24516,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="88" spans="1:55" ht="75" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:55" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>303</v>
       </c>
@@ -24667,7 +24669,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="89" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>312</v>
       </c>
@@ -24814,7 +24816,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="90" spans="1:55" ht="30" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:55" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>324</v>
       </c>
@@ -24966,7 +24968,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="91" spans="1:55" ht="30" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:55" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>325</v>
       </c>
@@ -25118,7 +25120,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="92" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>327</v>
       </c>
@@ -25273,7 +25275,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="93" spans="1:55" ht="30" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:55" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>335</v>
       </c>
@@ -25414,7 +25416,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="94" spans="1:55" ht="30" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:55" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>337</v>
       </c>
@@ -25567,7 +25569,7 @@
         <v>1021</v>
       </c>
     </row>
-    <row r="95" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>338</v>
       </c>
@@ -25722,7 +25724,7 @@
         <v>1021</v>
       </c>
     </row>
-    <row r="96" spans="1:55" ht="45" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:55" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>339</v>
       </c>
@@ -25877,7 +25879,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="97" spans="1:55" ht="45" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:55" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>342</v>
       </c>
@@ -26032,7 +26034,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="98" spans="1:55" ht="30" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:55" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>346</v>
       </c>
@@ -26187,7 +26189,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="99" spans="1:55" ht="45" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:55" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>347</v>
       </c>
@@ -26336,7 +26338,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="100" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>348</v>
       </c>
@@ -26479,7 +26481,7 @@
         <v>1577</v>
       </c>
     </row>
-    <row r="101" spans="1:55" ht="60" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:55" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>349</v>
       </c>
@@ -26635,7 +26637,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="102" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>352</v>
       </c>
@@ -26796,7 +26798,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="103" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>355</v>
       </c>
@@ -26951,7 +26953,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="104" spans="1:55" ht="75" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:55" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>362</v>
       </c>
@@ -27106,7 +27108,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="105" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>363</v>
       </c>
@@ -27261,7 +27263,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="106" spans="1:55" ht="45" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:55" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>367</v>
       </c>
@@ -27413,7 +27415,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="107" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>371</v>
       </c>
@@ -27574,7 +27576,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="108" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>372</v>
       </c>
@@ -27721,7 +27723,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="109" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>372</v>
       </c>
@@ -27868,7 +27870,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="110" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>372</v>
       </c>
@@ -28023,7 +28025,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="111" spans="1:55" ht="30" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:55" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>376</v>
       </c>
@@ -28178,7 +28180,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="112" spans="1:55" ht="30" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:55" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>378</v>
       </c>
@@ -28333,7 +28335,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="113" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>381</v>
       </c>
@@ -28479,7 +28481,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="114" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>384</v>
       </c>
@@ -28628,7 +28630,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="115" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>390</v>
       </c>
@@ -28772,7 +28774,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="116" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>400</v>
       </c>
@@ -28927,7 +28929,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="117" spans="1:55" ht="60" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:55" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>405</v>
       </c>
@@ -29088,7 +29090,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="118" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>408</v>
       </c>
@@ -29243,7 +29245,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="119" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>408</v>
       </c>
@@ -29380,7 +29382,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="120" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>412</v>
       </c>
@@ -29535,7 +29537,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="121" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>418</v>
       </c>
@@ -29694,7 +29696,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="122" spans="1:55" ht="30" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:55" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>419</v>
       </c>
@@ -29843,7 +29845,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="123" spans="1:55" ht="105" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:55" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>429</v>
       </c>
@@ -29998,7 +30000,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="124" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>430</v>
       </c>
@@ -30151,7 +30153,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="125" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>433</v>
       </c>
@@ -30306,7 +30308,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="126" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>438</v>
       </c>
@@ -30464,7 +30466,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="127" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>438</v>
       </c>
@@ -30595,7 +30597,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="128" spans="1:55" ht="30" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:55" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>441</v>
       </c>
@@ -30738,7 +30740,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="129" spans="1:55" ht="45" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:55" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>442</v>
       </c>
@@ -30882,7 +30884,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="130" spans="1:55" ht="60" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:55" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>452</v>
       </c>
@@ -31032,7 +31034,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="131" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>465</v>
       </c>
@@ -31181,7 +31183,7 @@
         <v>1067</v>
       </c>
     </row>
-    <row r="132" spans="1:55" ht="45" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:55" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>479</v>
       </c>
@@ -31336,7 +31338,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="133" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>482</v>
       </c>
@@ -31482,7 +31484,7 @@
         <v>1086</v>
       </c>
     </row>
-    <row r="134" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>486</v>
       </c>
@@ -31619,7 +31621,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="135" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>497</v>
       </c>
@@ -31771,7 +31773,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="136" spans="1:55" ht="30" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:55" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>498</v>
       </c>
@@ -32070,7 +32072,7 @@
         <v>2179</v>
       </c>
     </row>
-    <row r="138" spans="1:55" ht="45" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:55" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>517</v>
       </c>
@@ -32225,7 +32227,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="139" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>523</v>
       </c>
@@ -32369,7 +32371,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="140" spans="1:55" ht="30" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:55" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>524</v>
       </c>
@@ -32682,7 +32684,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="142" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>528</v>
       </c>
@@ -32834,7 +32836,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="143" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>531</v>
       </c>
@@ -32989,7 +32991,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="144" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <v>533</v>
       </c>
@@ -33144,7 +33146,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="145" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>536</v>
       </c>
@@ -33297,7 +33299,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="146" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>540</v>
       </c>
@@ -33452,7 +33454,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="147" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>545</v>
       </c>
@@ -33607,7 +33609,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="148" spans="1:55" ht="30" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:55" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>550</v>
       </c>
@@ -33757,7 +33759,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="149" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>553</v>
       </c>
@@ -33909,7 +33911,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="150" spans="1:55" ht="30" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:55" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>557</v>
       </c>
@@ -34064,7 +34066,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="151" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <v>558</v>
       </c>
@@ -34219,7 +34221,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="152" spans="1:55" ht="30" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:55" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>560</v>
       </c>
@@ -34368,7 +34370,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="153" spans="1:55" ht="30" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:55" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
         <v>561</v>
       </c>
@@ -34526,7 +34528,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="154" spans="1:55" ht="30" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:55" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <v>569</v>
       </c>
@@ -34681,7 +34683,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="155" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
         <v>569</v>
       </c>
@@ -34806,7 +34808,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="156" spans="1:55" ht="30" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:55" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <v>573</v>
       </c>
@@ -34962,7 +34964,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="157" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
         <v>574</v>
       </c>
@@ -35123,7 +35125,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="158" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
         <v>590</v>
       </c>
@@ -35269,7 +35271,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="159" spans="1:55" ht="30" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:55" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
         <v>600</v>
       </c>
@@ -35567,7 +35569,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="161" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
         <v>607</v>
       </c>
@@ -35683,7 +35685,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="162" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
         <v>612</v>
       </c>
@@ -35832,7 +35834,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="163" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
         <v>626</v>
       </c>
@@ -35987,7 +35989,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="164" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
         <v>627</v>
       </c>
@@ -36136,7 +36138,7 @@
         <v>1067</v>
       </c>
     </row>
-    <row r="165" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
         <v>628</v>
       </c>
@@ -36285,7 +36287,7 @@
         <v>1067</v>
       </c>
     </row>
-    <row r="166" spans="1:55" ht="30" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:55" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <v>636</v>
       </c>
@@ -36437,7 +36439,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="167" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
         <v>640</v>
       </c>
@@ -36592,7 +36594,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="168" spans="1:55" ht="45" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:55" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
         <v>648</v>
       </c>
@@ -36741,7 +36743,7 @@
         <v>1178</v>
       </c>
     </row>
-    <row r="169" spans="1:55" ht="30" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:55" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
         <v>649</v>
       </c>
@@ -36893,7 +36895,7 @@
         <v>1178</v>
       </c>
     </row>
-    <row r="170" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
         <v>650</v>
       </c>
@@ -37048,7 +37050,7 @@
         <v>1178</v>
       </c>
     </row>
-    <row r="171" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
         <v>659</v>
       </c>
@@ -37203,7 +37205,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="172" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
         <v>660</v>
       </c>
@@ -37358,7 +37360,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="173" spans="1:55" ht="30" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:55" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
         <v>672</v>
       </c>
@@ -37516,7 +37518,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="174" spans="1:55" ht="45" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:55" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
         <v>675</v>
       </c>
@@ -37669,7 +37671,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="175" spans="1:55" ht="30" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:55" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
         <v>676</v>
       </c>
@@ -37824,7 +37826,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="176" spans="1:55" ht="30" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:55" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
         <v>677</v>
       </c>
@@ -37979,7 +37981,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="177" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
         <v>678</v>
       </c>
@@ -38134,7 +38136,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="178" spans="1:55" ht="60" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:55" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
         <v>682</v>
       </c>
@@ -38289,7 +38291,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="179" spans="1:55" ht="30" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:55" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
         <v>684</v>
       </c>
@@ -38447,7 +38449,7 @@
         <v>1793</v>
       </c>
     </row>
-    <row r="180" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
         <v>685</v>
       </c>
@@ -38605,7 +38607,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="181" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
         <v>686</v>
       </c>
@@ -38760,7 +38762,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="182" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
         <v>687</v>
       </c>
@@ -38909,7 +38911,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="183" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:55" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
         <v>688</v>
       </c>
@@ -39064,7 +39066,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="184" spans="1:55" ht="30" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:55" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
         <v>689</v>
       </c>
@@ -39219,7 +39221,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="185" spans="1:55" ht="30" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:55" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
         <v>690</v>
       </c>
@@ -39380,7 +39382,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AK174"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
       <pane xSplit="1" topLeftCell="X1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="AA163" sqref="AA163"/>
     </sheetView>
@@ -39396,17 +39398,18 @@
     <col min="10" max="10" width="43.5703125" customWidth="1"/>
     <col min="11" max="11" width="16.5703125" customWidth="1"/>
     <col min="12" max="12" width="15.28515625" customWidth="1"/>
-    <col min="14" max="14" width="21.85546875" customWidth="1"/>
-    <col min="15" max="15" width="43.28515625" customWidth="1"/>
-    <col min="16" max="16" width="21.7109375" customWidth="1"/>
+    <col min="14" max="14" width="16.5703125" customWidth="1"/>
+    <col min="15" max="15" width="23.85546875" customWidth="1"/>
+    <col min="16" max="16" width="16.5703125" customWidth="1"/>
     <col min="17" max="17" width="17.5703125" customWidth="1"/>
     <col min="18" max="19" width="22" customWidth="1"/>
     <col min="20" max="20" width="21.42578125" customWidth="1"/>
     <col min="21" max="21" width="20" customWidth="1"/>
     <col min="22" max="22" width="18" customWidth="1"/>
-    <col min="23" max="24" width="37.28515625" customWidth="1"/>
+    <col min="23" max="23" width="26.85546875" customWidth="1"/>
+    <col min="24" max="24" width="24.85546875" customWidth="1"/>
     <col min="25" max="25" width="25" customWidth="1"/>
-    <col min="26" max="26" width="30" customWidth="1"/>
+    <col min="26" max="26" width="25.85546875" customWidth="1"/>
     <col min="27" max="27" width="64.42578125" customWidth="1"/>
     <col min="28" max="28" width="35.85546875" customWidth="1"/>
     <col min="29" max="29" width="37.140625" customWidth="1"/>
@@ -45767,7 +45770,7 @@
       <c r="V60" s="1">
         <v>1</v>
       </c>
-      <c r="W60" s="12" t="s">
+      <c r="W60" s="1" t="s">
         <v>2310</v>
       </c>
       <c r="X60" s="1">
@@ -54284,9 +54287,7 @@
       <c r="L141" s="1">
         <v>20</v>
       </c>
-      <c r="M141" s="1">
-        <v>4</v>
-      </c>
+      <c r="M141" s="1"/>
       <c r="N141" s="1" t="s">
         <v>2268</v>
       </c>
@@ -54318,9 +54319,7 @@
       <c r="X141" s="1"/>
       <c r="Y141" s="1"/>
       <c r="Z141" s="1"/>
-      <c r="AA141" s="1" t="s">
-        <v>2797</v>
-      </c>
+      <c r="AA141" s="1"/>
       <c r="AB141" s="1" t="s">
         <v>39</v>
       </c>

</xml_diff>

<commit_message>
added results for technologies
</commit_message>
<xml_diff>
--- a/data/raw/Review_data_all_packages.xlsx
+++ b/data/raw/Review_data_all_packages.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neleb\Documents\GitHub\CSE-review\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F573F52D-6E39-40F1-BDA8-6802463AE903}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2213437B-B1F8-4C8E-8540-9AEC103360AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10014" uniqueCount="2828">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10014" uniqueCount="2827">
   <si>
     <t>id</t>
   </si>
@@ -8992,15 +8992,9 @@
     <t>not_specified; facebook</t>
   </si>
   <si>
-    <t>not specified; computer</t>
-  </si>
-  <si>
     <t>mobile_device; computer</t>
   </si>
   <si>
-    <t>computer; workplace IT</t>
-  </si>
-  <si>
     <t>not_specified; mobile_device</t>
   </si>
   <si>
@@ -9053,6 +9047,9 @@
   </si>
   <si>
     <t>smartphone; mobile_app</t>
+  </si>
+  <si>
+    <t>computer; workplace_IT</t>
   </si>
 </sst>
 </file>
@@ -11337,8 +11334,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BD185"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R166" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V181" sqref="V181"/>
+    <sheetView tabSelected="1" topLeftCell="R104" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V115" sqref="V115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17164,7 +17161,7 @@
         <v>0</v>
       </c>
       <c r="V38" s="1" t="s">
-        <v>2807</v>
+        <v>2800</v>
       </c>
       <c r="W38" s="1">
         <v>1</v>
@@ -18409,7 +18406,7 @@
         <v>0</v>
       </c>
       <c r="V46" s="1" t="s">
-        <v>2808</v>
+        <v>2807</v>
       </c>
       <c r="W46" s="1">
         <v>1</v>
@@ -18564,7 +18561,7 @@
         <v>0</v>
       </c>
       <c r="V47" s="1" t="s">
-        <v>2807</v>
+        <v>2800</v>
       </c>
       <c r="W47" s="1">
         <v>1</v>
@@ -19498,7 +19495,7 @@
         <v>0</v>
       </c>
       <c r="V53" s="1" t="s">
-        <v>2809</v>
+        <v>2826</v>
       </c>
       <c r="W53" s="1">
         <v>0</v>
@@ -20751,7 +20748,7 @@
         <v>0</v>
       </c>
       <c r="V61" s="1" t="s">
-        <v>2822</v>
+        <v>2820</v>
       </c>
       <c r="W61" s="1">
         <v>1</v>
@@ -21673,7 +21670,7 @@
         <v>0</v>
       </c>
       <c r="V67" s="1" t="s">
-        <v>2807</v>
+        <v>2800</v>
       </c>
       <c r="W67" s="1">
         <v>1</v>
@@ -23696,7 +23693,7 @@
         <v>0</v>
       </c>
       <c r="V80" s="1" t="s">
-        <v>2810</v>
+        <v>2808</v>
       </c>
       <c r="W80" s="1">
         <v>1</v>
@@ -23846,7 +23843,7 @@
         <v>0</v>
       </c>
       <c r="V81" s="1" t="s">
-        <v>2811</v>
+        <v>2809</v>
       </c>
       <c r="W81" s="1">
         <v>1</v>
@@ -24473,7 +24470,7 @@
         <v>0</v>
       </c>
       <c r="V85" s="1" t="s">
-        <v>2812</v>
+        <v>2810</v>
       </c>
       <c r="W85" s="1">
         <v>1</v>
@@ -25246,7 +25243,7 @@
         <v>0</v>
       </c>
       <c r="V90" s="1" t="s">
-        <v>2813</v>
+        <v>2811</v>
       </c>
       <c r="W90" s="1">
         <v>1</v>
@@ -25401,7 +25398,7 @@
         <v>0</v>
       </c>
       <c r="V91" s="1" t="s">
-        <v>2823</v>
+        <v>2821</v>
       </c>
       <c r="W91" s="1">
         <v>1</v>
@@ -25711,7 +25708,7 @@
         <v>0</v>
       </c>
       <c r="V93" s="1" t="s">
-        <v>2824</v>
+        <v>2822</v>
       </c>
       <c r="W93" s="1">
         <v>1</v>
@@ -26330,7 +26327,7 @@
         <v>0</v>
       </c>
       <c r="V97" s="1" t="s">
-        <v>2809</v>
+        <v>2826</v>
       </c>
       <c r="W97" s="1">
         <v>1</v>
@@ -26944,7 +26941,7 @@
         <v>0</v>
       </c>
       <c r="V101" s="1" t="s">
-        <v>2808</v>
+        <v>2807</v>
       </c>
       <c r="W101" s="1">
         <v>1</v>
@@ -27267,7 +27264,7 @@
         <v>0</v>
       </c>
       <c r="V103" s="1" t="s">
-        <v>2807</v>
+        <v>2800</v>
       </c>
       <c r="W103" s="1">
         <v>1</v>
@@ -28210,7 +28207,7 @@
         <v>0</v>
       </c>
       <c r="V109" s="1" t="s">
-        <v>2814</v>
+        <v>2812</v>
       </c>
       <c r="W109" s="1">
         <v>1</v>
@@ -28360,7 +28357,7 @@
         <v>0</v>
       </c>
       <c r="V110" s="1" t="s">
-        <v>2814</v>
+        <v>2812</v>
       </c>
       <c r="W110" s="1">
         <v>1</v>
@@ -28676,7 +28673,7 @@
         <v>0</v>
       </c>
       <c r="V112" s="1" t="s">
-        <v>2808</v>
+        <v>2807</v>
       </c>
       <c r="W112" s="1">
         <v>1</v>
@@ -28983,7 +28980,7 @@
         <v>0</v>
       </c>
       <c r="V114" s="1" t="s">
-        <v>2809</v>
+        <v>2826</v>
       </c>
       <c r="W114" s="1">
         <v>1</v>
@@ -29135,7 +29132,7 @@
         <v>39</v>
       </c>
       <c r="V115" s="1" t="s">
-        <v>2809</v>
+        <v>2826</v>
       </c>
       <c r="W115" s="1" t="s">
         <v>39</v>
@@ -29440,7 +29437,7 @@
         <v>0</v>
       </c>
       <c r="V117" s="1" t="s">
-        <v>2825</v>
+        <v>2823</v>
       </c>
       <c r="W117" s="1">
         <v>1</v>
@@ -30060,7 +30057,7 @@
         <v>0</v>
       </c>
       <c r="V121" s="1" t="s">
-        <v>2807</v>
+        <v>2800</v>
       </c>
       <c r="W121" s="1">
         <v>0</v>
@@ -30222,7 +30219,7 @@
         <v>0</v>
       </c>
       <c r="V122" s="1" t="s">
-        <v>2808</v>
+        <v>2807</v>
       </c>
       <c r="W122" s="1">
         <v>1</v>
@@ -30374,7 +30371,7 @@
         <v>1</v>
       </c>
       <c r="V123" s="1" t="s">
-        <v>2826</v>
+        <v>2824</v>
       </c>
       <c r="W123" s="1">
         <v>1</v>
@@ -31141,7 +31138,7 @@
         <v>0</v>
       </c>
       <c r="V128" s="1" t="s">
-        <v>2811</v>
+        <v>2809</v>
       </c>
       <c r="W128" s="1">
         <v>1</v>
@@ -31587,7 +31584,7 @@
         <v>0</v>
       </c>
       <c r="V131" s="1" t="s">
-        <v>2807</v>
+        <v>2800</v>
       </c>
       <c r="W131" s="1">
         <v>1</v>
@@ -31897,7 +31894,7 @@
         <v>0</v>
       </c>
       <c r="V133" s="1" t="s">
-        <v>2815</v>
+        <v>2813</v>
       </c>
       <c r="W133" s="1">
         <v>1</v>
@@ -32494,7 +32491,7 @@
         <v>0</v>
       </c>
       <c r="V137" s="1" t="s">
-        <v>2816</v>
+        <v>2814</v>
       </c>
       <c r="W137" s="1">
         <v>0</v>
@@ -33106,7 +33103,7 @@
         <v>0</v>
       </c>
       <c r="V141" s="1" t="s">
-        <v>2817</v>
+        <v>2815</v>
       </c>
       <c r="W141" s="1">
         <v>0</v>
@@ -33580,7 +33577,7 @@
         <v>0</v>
       </c>
       <c r="V144" s="1" t="s">
-        <v>2808</v>
+        <v>2807</v>
       </c>
       <c r="W144" s="1">
         <v>1</v>
@@ -34210,7 +34207,7 @@
         <v>0</v>
       </c>
       <c r="V148" s="1" t="s">
-        <v>2818</v>
+        <v>2816</v>
       </c>
       <c r="W148" s="1">
         <v>1</v>
@@ -34986,7 +34983,7 @@
         <v>0</v>
       </c>
       <c r="V153" s="1" t="s">
-        <v>2808</v>
+        <v>2807</v>
       </c>
       <c r="W153" s="1">
         <v>1</v>
@@ -36057,7 +36054,7 @@
         <v>0</v>
       </c>
       <c r="V160" s="1" t="s">
-        <v>2808</v>
+        <v>2807</v>
       </c>
       <c r="W160" s="1">
         <v>0</v>
@@ -36200,7 +36197,7 @@
         <v>815</v>
       </c>
       <c r="V161" s="1" t="s">
-        <v>2808</v>
+        <v>2807</v>
       </c>
       <c r="X161" s="1" t="s">
         <v>2018</v>
@@ -36790,7 +36787,7 @@
         <v>0</v>
       </c>
       <c r="V165" s="1" t="s">
-        <v>2819</v>
+        <v>2817</v>
       </c>
       <c r="W165" s="1">
         <v>1</v>
@@ -37097,7 +37094,7 @@
         <v>0</v>
       </c>
       <c r="V167" s="1" t="s">
-        <v>2813</v>
+        <v>2811</v>
       </c>
       <c r="W167" s="1">
         <v>1</v>
@@ -38827,7 +38824,7 @@
         <v>0</v>
       </c>
       <c r="V178" s="1" t="s">
-        <v>2820</v>
+        <v>2818</v>
       </c>
       <c r="W178" s="1">
         <v>1</v>
@@ -39146,7 +39143,7 @@
         <v>0</v>
       </c>
       <c r="V180" s="1" t="s">
-        <v>2819</v>
+        <v>2817</v>
       </c>
       <c r="W180" s="1">
         <v>1</v>
@@ -39465,7 +39462,7 @@
         <v>0</v>
       </c>
       <c r="V182" s="1" t="s">
-        <v>2811</v>
+        <v>2809</v>
       </c>
       <c r="W182" s="1">
         <v>1</v>
@@ -39933,7 +39930,7 @@
         <v>0</v>
       </c>
       <c r="V185" s="1" t="s">
-        <v>2827</v>
+        <v>2825</v>
       </c>
       <c r="W185" s="1">
         <v>1</v>
@@ -58656,7 +58653,7 @@
     </row>
     <row r="27" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>2821</v>
+        <v>2819</v>
       </c>
     </row>
     <row r="28" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>